<commit_message>
dada updated and covid III refitted
</commit_message>
<xml_diff>
--- a/COVID_EXCEL/COVID III.xlsx
+++ b/COVID_EXCEL/COVID III.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\u093799\Documents\GitHub\COVID-19\COVID_EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E0B93B-6B02-40BA-BD93-4C62736CC7DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1433DF-B806-4C64-99BC-4500DDC79CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{4377578F-4DE2-4D7D-A4C8-86901BC845F0}"/>
   </bookViews>
@@ -574,34 +574,43 @@
                   <c:v>491</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>530</c:v>
+                  <c:v>529</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>572</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>617</c:v>
+                  <c:v>613</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>666</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>718</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>775</c:v>
+                  <c:v>766</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>836</c:v>
+                  <c:v>825</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>902</c:v>
+                  <c:v>888</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>974</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1051</c:v>
+                  <c:v>1029</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1193</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -985,6 +994,15 @@
                 <c:pt idx="44">
                   <c:v>1049</c:v>
                 </c:pt>
+                <c:pt idx="45">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1284</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1233,199 +1251,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="65"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>52</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>61</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>66</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>71</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>77</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>84</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>91</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>98</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>106</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>115</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>124</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>135</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>146</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>158</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>171</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>185</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>201</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>217</c:v>
+                  <c:v>227</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>235</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>254</c:v>
+                  <c:v>263</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>275</c:v>
+                  <c:v>283</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>298</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>323</c:v>
+                  <c:v>328</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>350</c:v>
+                  <c:v>353</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>379</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>410</c:v>
+                  <c:v>409</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>444</c:v>
+                  <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>481</c:v>
+                  <c:v>473</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>521</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>565</c:v>
+                  <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>612</c:v>
+                  <c:v>591</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>663</c:v>
+                  <c:v>637</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>718</c:v>
+                  <c:v>686</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>778</c:v>
+                  <c:v>739</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>843</c:v>
+                  <c:v>795</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>913</c:v>
+                  <c:v>856</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>989</c:v>
+                  <c:v>922</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1072</c:v>
+                  <c:v>993</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1162</c:v>
+                  <c:v>1069</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1259</c:v>
+                  <c:v>1151</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1364</c:v>
+                  <c:v>1239</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1477</c:v>
+                  <c:v>1334</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1600</c:v>
+                  <c:v>1436</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1734</c:v>
+                  <c:v>1546</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1878</c:v>
+                  <c:v>1664</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2034</c:v>
+                  <c:v>1791</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2203</c:v>
+                  <c:v>1929</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2386</c:v>
+                  <c:v>2077</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2585</c:v>
+                  <c:v>2236</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2801</c:v>
+                  <c:v>2408</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3035</c:v>
+                  <c:v>2592</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3288</c:v>
+                  <c:v>2791</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3562</c:v>
+                  <c:v>3004</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3859</c:v>
+                  <c:v>3235</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4180</c:v>
+                  <c:v>3482</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4528</c:v>
+                  <c:v>3749</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4905</c:v>
+                  <c:v>4037</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5313</c:v>
+                  <c:v>4347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2446,34 +2464,43 @@
                   <c:v>491</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>530</c:v>
+                  <c:v>529</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>572</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>617</c:v>
+                  <c:v>613</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>666</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>718</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>775</c:v>
+                  <c:v>766</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>836</c:v>
+                  <c:v>825</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>902</c:v>
+                  <c:v>888</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>974</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1051</c:v>
+                  <c:v>1029</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1193</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3239,6 +3266,15 @@
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>1049</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4227,34 +4263,43 @@
                   <c:v>491</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>530</c:v>
+                  <c:v>529</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>572</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>617</c:v>
+                  <c:v>613</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>666</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>718</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>775</c:v>
+                  <c:v>766</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>836</c:v>
+                  <c:v>825</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>902</c:v>
+                  <c:v>888</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>974</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1051</c:v>
+                  <c:v>1029</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1193</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4980,6 +5025,15 @@
                 <c:pt idx="108">
                   <c:v>1049</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1284</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5377,28 +5431,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="115"/>
                 <c:pt idx="107">
-                  <c:v>974</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1051</c:v>
+                  <c:v>1029</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1134</c:v>
+                  <c:v>1108</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1223</c:v>
+                  <c:v>1193</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1320</c:v>
+                  <c:v>1285</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1424</c:v>
+                  <c:v>1384</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1536</c:v>
+                  <c:v>1490</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1658</c:v>
+                  <c:v>1604</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6408,34 +6462,43 @@
                   <c:v>491</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>530</c:v>
+                  <c:v>529</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>572</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>617</c:v>
+                  <c:v>613</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>666</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>718</c:v>
+                  <c:v>711</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>775</c:v>
+                  <c:v>766</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>836</c:v>
+                  <c:v>825</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>902</c:v>
+                  <c:v>888</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>974</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1051</c:v>
+                  <c:v>1029</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1108</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1193</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7182,6 +7245,15 @@
                 <c:pt idx="108">
                   <c:v>1049</c:v>
                 </c:pt>
+                <c:pt idx="109">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1284</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7601,49 +7673,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="122"/>
                 <c:pt idx="107">
-                  <c:v>974</c:v>
+                  <c:v>956</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1051</c:v>
+                  <c:v>1029</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1134</c:v>
+                  <c:v>1108</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1223</c:v>
+                  <c:v>1193</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1320</c:v>
+                  <c:v>1285</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1424</c:v>
+                  <c:v>1384</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1536</c:v>
+                  <c:v>1490</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1658</c:v>
+                  <c:v>1604</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1769</c:v>
+                  <c:v>1711</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1887</c:v>
+                  <c:v>1825</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2013</c:v>
+                  <c:v>1947</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2147</c:v>
+                  <c:v>2077</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2290</c:v>
+                  <c:v>2215</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2442</c:v>
+                  <c:v>2362</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2604</c:v>
+                  <c:v>2519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10536,10 +10608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ECC772-9D54-48D6-A63B-745C3F43084A}">
-  <dimension ref="A2:K113"/>
+  <dimension ref="A2:K114"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111:A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11450,6 +11522,14 @@
         <v>1208</v>
       </c>
     </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>44130</v>
+      </c>
+      <c r="B114">
+        <v>1284</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11460,8 +11540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF8076A-EB14-4DFF-97BA-E5541A25D5B9}">
   <dimension ref="A1:P134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S19" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105:C120"/>
+    <sheetView tabSelected="1" topLeftCell="K101" workbookViewId="0">
+      <selection activeCell="W118" sqref="W118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11475,7 +11555,7 @@
         <v>2</v>
       </c>
       <c r="D1">
-        <v>2</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -13664,7 +13744,7 @@
         <v>68</v>
       </c>
       <c r="I54" s="4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K54" s="1">
         <f t="shared" si="1"/>
@@ -13679,8 +13759,8 @@
         <v>65</v>
       </c>
       <c r="P54">
-        <f>I54</f>
-        <v>10</v>
+        <f t="shared" ref="P54:P118" si="11">I54</f>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -13714,8 +13794,8 @@
         <v>69</v>
       </c>
       <c r="I55" s="4">
-        <f t="shared" ref="I55:I111" si="11">I54+ROUND(($D$1/$D$2)*G54*(I54/$D$3),0)-ROUND(I54/$D$2,0)</f>
-        <v>11</v>
+        <f t="shared" ref="I55:I111" si="12">I54+ROUND(($D$1/$D$2)*G54*(I54/$D$3),0)-ROUND(I54/$D$2,0)</f>
+        <v>14</v>
       </c>
       <c r="K55" s="1">
         <f t="shared" si="1"/>
@@ -13730,8 +13810,8 @@
         <v>66</v>
       </c>
       <c r="P55">
-        <f t="shared" ref="P55:P118" si="12">I55</f>
-        <v>11</v>
+        <f t="shared" si="11"/>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -13765,8 +13845,8 @@
         <v>70</v>
       </c>
       <c r="I56" s="4">
-        <f t="shared" si="11"/>
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>15</v>
       </c>
       <c r="K56" s="1">
         <f t="shared" si="1"/>
@@ -13781,8 +13861,8 @@
         <v>69</v>
       </c>
       <c r="P56">
-        <f t="shared" si="12"/>
-        <v>12</v>
+        <f t="shared" si="11"/>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -13816,8 +13896,8 @@
         <v>72</v>
       </c>
       <c r="I57" s="4">
-        <f t="shared" si="11"/>
-        <v>13</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="K57" s="1">
         <f t="shared" si="1"/>
@@ -13832,8 +13912,8 @@
         <v>67</v>
       </c>
       <c r="P57">
-        <f t="shared" si="12"/>
-        <v>13</v>
+        <f t="shared" si="11"/>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -13867,8 +13947,8 @@
         <v>77</v>
       </c>
       <c r="I58" s="4">
-        <f t="shared" si="11"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>18</v>
       </c>
       <c r="K58" s="1">
         <f t="shared" si="1"/>
@@ -13883,8 +13963,8 @@
         <v>74</v>
       </c>
       <c r="P58">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="11"/>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -13918,8 +13998,8 @@
         <v>83</v>
       </c>
       <c r="I59" s="4">
-        <f t="shared" si="11"/>
-        <v>15</v>
+        <f t="shared" si="12"/>
+        <v>19</v>
       </c>
       <c r="K59" s="1">
         <f t="shared" si="1"/>
@@ -13934,8 +14014,8 @@
         <v>79</v>
       </c>
       <c r="P59">
-        <f t="shared" si="12"/>
-        <v>15</v>
+        <f t="shared" si="11"/>
+        <v>19</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -13969,8 +14049,8 @@
         <v>88</v>
       </c>
       <c r="I60" s="4">
-        <f t="shared" si="11"/>
-        <v>16</v>
+        <f t="shared" si="12"/>
+        <v>20</v>
       </c>
       <c r="K60" s="1">
         <f t="shared" si="1"/>
@@ -13985,8 +14065,8 @@
         <v>86</v>
       </c>
       <c r="P60">
-        <f t="shared" si="12"/>
-        <v>16</v>
+        <f t="shared" si="11"/>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -14020,8 +14100,8 @@
         <v>94</v>
       </c>
       <c r="I61" s="4">
-        <f t="shared" si="11"/>
-        <v>18</v>
+        <f t="shared" si="12"/>
+        <v>21</v>
       </c>
       <c r="K61" s="1">
         <f t="shared" si="1"/>
@@ -14036,8 +14116,8 @@
         <v>94</v>
       </c>
       <c r="P61">
-        <f t="shared" si="12"/>
-        <v>18</v>
+        <f t="shared" si="11"/>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -14071,8 +14151,8 @@
         <v>100</v>
       </c>
       <c r="I62" s="4">
-        <f t="shared" si="11"/>
-        <v>19</v>
+        <f t="shared" si="12"/>
+        <v>22</v>
       </c>
       <c r="K62" s="1">
         <f t="shared" si="1"/>
@@ -14087,8 +14167,8 @@
         <v>107</v>
       </c>
       <c r="P62">
-        <f t="shared" si="12"/>
-        <v>19</v>
+        <f t="shared" si="11"/>
+        <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -14122,8 +14202,8 @@
         <v>107</v>
       </c>
       <c r="I63" s="4">
-        <f t="shared" si="11"/>
-        <v>20</v>
+        <f t="shared" si="12"/>
+        <v>24</v>
       </c>
       <c r="K63" s="1">
         <f t="shared" si="1"/>
@@ -14138,8 +14218,8 @@
         <v>109</v>
       </c>
       <c r="P63">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f t="shared" si="11"/>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -14173,8 +14253,8 @@
         <v>114</v>
       </c>
       <c r="I64" s="4">
-        <f t="shared" si="11"/>
-        <v>21</v>
+        <f t="shared" si="12"/>
+        <v>26</v>
       </c>
       <c r="K64" s="1">
         <f t="shared" si="1"/>
@@ -14189,8 +14269,8 @@
         <v>120</v>
       </c>
       <c r="P64">
-        <f t="shared" si="12"/>
-        <v>21</v>
+        <f t="shared" si="11"/>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -14224,8 +14304,8 @@
         <v>121</v>
       </c>
       <c r="I65" s="4">
-        <f t="shared" si="11"/>
-        <v>22</v>
+        <f t="shared" si="12"/>
+        <v>28</v>
       </c>
       <c r="K65" s="1">
         <f t="shared" si="1"/>
@@ -14240,8 +14320,8 @@
         <v>121</v>
       </c>
       <c r="P65">
-        <f t="shared" si="12"/>
-        <v>22</v>
+        <f t="shared" si="11"/>
+        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -14275,8 +14355,8 @@
         <v>129</v>
       </c>
       <c r="I66" s="4">
-        <f t="shared" si="11"/>
-        <v>24</v>
+        <f t="shared" si="12"/>
+        <v>30</v>
       </c>
       <c r="K66" s="1">
         <f t="shared" si="1"/>
@@ -14291,8 +14371,8 @@
         <v>121</v>
       </c>
       <c r="P66">
-        <f t="shared" si="12"/>
-        <v>24</v>
+        <f t="shared" si="11"/>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -14326,8 +14406,8 @@
         <v>137</v>
       </c>
       <c r="I67" s="4">
-        <f t="shared" si="11"/>
-        <v>26</v>
+        <f t="shared" si="12"/>
+        <v>32</v>
       </c>
       <c r="K67" s="1">
         <f t="shared" si="1"/>
@@ -14342,8 +14422,8 @@
         <v>133</v>
       </c>
       <c r="P67">
-        <f t="shared" si="12"/>
-        <v>26</v>
+        <f t="shared" si="11"/>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -14377,8 +14457,8 @@
         <v>147</v>
       </c>
       <c r="I68" s="4">
-        <f t="shared" si="11"/>
-        <v>28</v>
+        <f t="shared" si="12"/>
+        <v>34</v>
       </c>
       <c r="K68" s="1">
         <f t="shared" si="1"/>
@@ -14393,8 +14473,8 @@
         <v>142</v>
       </c>
       <c r="P68">
-        <f t="shared" si="12"/>
-        <v>28</v>
+        <f t="shared" si="11"/>
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -14428,8 +14508,8 @@
         <v>157</v>
       </c>
       <c r="I69" s="4">
-        <f t="shared" si="11"/>
-        <v>31</v>
+        <f t="shared" si="12"/>
+        <v>36</v>
       </c>
       <c r="K69" s="1">
         <f t="shared" si="1"/>
@@ -14444,8 +14524,8 @@
         <v>143</v>
       </c>
       <c r="P69">
-        <f t="shared" si="12"/>
-        <v>31</v>
+        <f t="shared" si="11"/>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -14479,8 +14559,8 @@
         <v>162</v>
       </c>
       <c r="I70" s="4">
-        <f t="shared" si="11"/>
-        <v>33</v>
+        <f t="shared" si="12"/>
+        <v>39</v>
       </c>
       <c r="K70" s="1">
         <f t="shared" si="1"/>
@@ -14495,8 +14575,8 @@
         <v>150</v>
       </c>
       <c r="P70">
-        <f t="shared" si="12"/>
-        <v>33</v>
+        <f t="shared" si="11"/>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -14530,8 +14610,8 @@
         <v>167</v>
       </c>
       <c r="I71" s="4">
-        <f t="shared" si="11"/>
-        <v>35</v>
+        <f t="shared" si="12"/>
+        <v>42</v>
       </c>
       <c r="K71" s="1">
         <f t="shared" ref="K71:K134" si="13">A71</f>
@@ -14546,8 +14626,8 @@
         <v>164</v>
       </c>
       <c r="P71">
-        <f t="shared" si="12"/>
-        <v>35</v>
+        <f t="shared" si="11"/>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -14581,8 +14661,8 @@
         <v>172</v>
       </c>
       <c r="I72" s="4">
-        <f t="shared" si="11"/>
-        <v>38</v>
+        <f t="shared" si="12"/>
+        <v>45</v>
       </c>
       <c r="K72" s="1">
         <f t="shared" si="13"/>
@@ -14597,8 +14677,8 @@
         <v>175</v>
       </c>
       <c r="P72">
-        <f t="shared" si="12"/>
-        <v>38</v>
+        <f t="shared" si="11"/>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -14632,8 +14712,8 @@
         <v>178</v>
       </c>
       <c r="I73" s="4">
-        <f t="shared" si="11"/>
-        <v>41</v>
+        <f t="shared" si="12"/>
+        <v>48</v>
       </c>
       <c r="K73" s="1">
         <f t="shared" si="13"/>
@@ -14648,8 +14728,8 @@
         <v>182</v>
       </c>
       <c r="P73">
-        <f t="shared" si="12"/>
-        <v>41</v>
+        <f t="shared" si="11"/>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -14683,8 +14763,8 @@
         <v>184</v>
       </c>
       <c r="I74" s="4">
-        <f t="shared" si="11"/>
-        <v>45</v>
+        <f t="shared" si="12"/>
+        <v>52</v>
       </c>
       <c r="K74" s="1">
         <f t="shared" si="13"/>
@@ -14699,8 +14779,8 @@
         <v>187</v>
       </c>
       <c r="P74">
-        <f t="shared" si="12"/>
-        <v>45</v>
+        <f t="shared" si="11"/>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -14734,8 +14814,8 @@
         <v>190</v>
       </c>
       <c r="I75" s="4">
-        <f t="shared" si="11"/>
-        <v>48</v>
+        <f t="shared" si="12"/>
+        <v>56</v>
       </c>
       <c r="K75" s="1">
         <f t="shared" si="13"/>
@@ -14750,8 +14830,8 @@
         <v>197</v>
       </c>
       <c r="P75">
-        <f t="shared" si="12"/>
-        <v>48</v>
+        <f t="shared" si="11"/>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -14785,8 +14865,8 @@
         <v>196</v>
       </c>
       <c r="I76" s="4">
-        <f t="shared" si="11"/>
-        <v>52</v>
+        <f t="shared" si="12"/>
+        <v>60</v>
       </c>
       <c r="K76" s="1">
         <f t="shared" si="13"/>
@@ -14801,8 +14881,8 @@
         <v>201</v>
       </c>
       <c r="P76">
-        <f t="shared" si="12"/>
-        <v>52</v>
+        <f t="shared" si="11"/>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -14836,8 +14916,8 @@
         <v>203</v>
       </c>
       <c r="I77" s="4">
-        <f t="shared" si="11"/>
-        <v>57</v>
+        <f t="shared" si="12"/>
+        <v>65</v>
       </c>
       <c r="K77" s="1">
         <f t="shared" si="13"/>
@@ -14852,8 +14932,8 @@
         <v>207</v>
       </c>
       <c r="P77">
-        <f t="shared" si="12"/>
-        <v>57</v>
+        <f t="shared" si="11"/>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -14887,8 +14967,8 @@
         <v>210</v>
       </c>
       <c r="I78" s="4">
-        <f t="shared" si="11"/>
-        <v>61</v>
+        <f t="shared" si="12"/>
+        <v>70</v>
       </c>
       <c r="K78" s="1">
         <f t="shared" si="13"/>
@@ -14903,8 +14983,8 @@
         <v>212</v>
       </c>
       <c r="P78">
-        <f t="shared" si="12"/>
-        <v>61</v>
+        <f t="shared" si="11"/>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -14938,8 +15018,8 @@
         <v>216</v>
       </c>
       <c r="I79" s="4">
-        <f t="shared" si="11"/>
-        <v>66</v>
+        <f t="shared" si="12"/>
+        <v>75</v>
       </c>
       <c r="K79" s="1">
         <f t="shared" si="13"/>
@@ -14954,8 +15034,8 @@
         <v>208</v>
       </c>
       <c r="P79">
-        <f t="shared" si="12"/>
-        <v>66</v>
+        <f t="shared" si="11"/>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -14989,8 +15069,8 @@
         <v>223</v>
       </c>
       <c r="I80" s="4">
-        <f t="shared" si="11"/>
-        <v>71</v>
+        <f t="shared" si="12"/>
+        <v>81</v>
       </c>
       <c r="K80" s="1">
         <f t="shared" si="13"/>
@@ -15005,8 +15085,8 @@
         <v>215</v>
       </c>
       <c r="P80">
-        <f t="shared" si="12"/>
-        <v>71</v>
+        <f t="shared" si="11"/>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -15040,8 +15120,8 @@
         <v>230</v>
       </c>
       <c r="I81" s="4">
-        <f t="shared" si="11"/>
-        <v>77</v>
+        <f t="shared" si="12"/>
+        <v>87</v>
       </c>
       <c r="K81" s="1">
         <f t="shared" si="13"/>
@@ -15056,8 +15136,8 @@
         <v>222</v>
       </c>
       <c r="P81">
-        <f t="shared" si="12"/>
-        <v>77</v>
+        <f t="shared" si="11"/>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -15091,8 +15171,8 @@
         <v>238</v>
       </c>
       <c r="I82" s="4">
-        <f t="shared" si="11"/>
-        <v>84</v>
+        <f t="shared" si="12"/>
+        <v>94</v>
       </c>
       <c r="K82" s="1">
         <f t="shared" si="13"/>
@@ -15107,8 +15187,8 @@
         <v>232</v>
       </c>
       <c r="P82">
-        <f t="shared" si="12"/>
-        <v>84</v>
+        <f t="shared" si="11"/>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -15142,8 +15222,8 @@
         <v>246</v>
       </c>
       <c r="I83" s="4">
-        <f t="shared" si="11"/>
-        <v>91</v>
+        <f t="shared" si="12"/>
+        <v>101</v>
       </c>
       <c r="K83" s="1">
         <f t="shared" si="13"/>
@@ -15158,8 +15238,8 @@
         <v>239</v>
       </c>
       <c r="P83">
-        <f t="shared" si="12"/>
-        <v>91</v>
+        <f t="shared" si="11"/>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -15193,8 +15273,8 @@
         <v>254</v>
       </c>
       <c r="I84" s="4">
-        <f t="shared" si="11"/>
-        <v>98</v>
+        <f t="shared" si="12"/>
+        <v>109</v>
       </c>
       <c r="K84" s="1">
         <f t="shared" si="13"/>
@@ -15209,8 +15289,8 @@
         <v>244</v>
       </c>
       <c r="P84">
-        <f t="shared" si="12"/>
-        <v>98</v>
+        <f t="shared" si="11"/>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -15244,8 +15324,8 @@
         <v>258</v>
       </c>
       <c r="I85" s="4">
-        <f t="shared" si="11"/>
-        <v>106</v>
+        <f t="shared" si="12"/>
+        <v>117</v>
       </c>
       <c r="K85" s="1">
         <f t="shared" si="13"/>
@@ -15260,8 +15340,8 @@
         <v>246</v>
       </c>
       <c r="P85">
-        <f t="shared" si="12"/>
-        <v>106</v>
+        <f t="shared" si="11"/>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -15295,8 +15375,8 @@
         <v>262</v>
       </c>
       <c r="I86" s="4">
-        <f t="shared" si="11"/>
-        <v>115</v>
+        <f t="shared" si="12"/>
+        <v>126</v>
       </c>
       <c r="K86" s="1">
         <f t="shared" si="13"/>
@@ -15311,8 +15391,8 @@
         <v>244</v>
       </c>
       <c r="P86">
-        <f t="shared" si="12"/>
-        <v>115</v>
+        <f t="shared" si="11"/>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -15346,8 +15426,8 @@
         <v>266</v>
       </c>
       <c r="I87" s="4">
-        <f t="shared" si="11"/>
-        <v>124</v>
+        <f t="shared" si="12"/>
+        <v>135</v>
       </c>
       <c r="K87" s="1">
         <f t="shared" si="13"/>
@@ -15362,8 +15442,8 @@
         <v>247</v>
       </c>
       <c r="P87">
-        <f t="shared" si="12"/>
-        <v>124</v>
+        <f t="shared" si="11"/>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -15397,8 +15477,8 @@
         <v>271</v>
       </c>
       <c r="I88" s="4">
-        <f t="shared" si="11"/>
-        <v>135</v>
+        <f t="shared" si="12"/>
+        <v>146</v>
       </c>
       <c r="K88" s="1">
         <f t="shared" si="13"/>
@@ -15413,8 +15493,8 @@
         <v>254</v>
       </c>
       <c r="P88">
-        <f t="shared" si="12"/>
-        <v>135</v>
+        <f t="shared" si="11"/>
+        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -15448,8 +15528,8 @@
         <v>275</v>
       </c>
       <c r="I89" s="4">
-        <f t="shared" si="11"/>
-        <v>146</v>
+        <f t="shared" si="12"/>
+        <v>157</v>
       </c>
       <c r="K89" s="1">
         <f t="shared" si="13"/>
@@ -15464,8 +15544,8 @@
         <v>264</v>
       </c>
       <c r="P89">
-        <f t="shared" si="12"/>
-        <v>146</v>
+        <f t="shared" si="11"/>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -15499,8 +15579,8 @@
         <v>279</v>
       </c>
       <c r="I90" s="4">
-        <f t="shared" si="11"/>
-        <v>158</v>
+        <f t="shared" si="12"/>
+        <v>169</v>
       </c>
       <c r="K90" s="1">
         <f t="shared" si="13"/>
@@ -15515,8 +15595,8 @@
         <v>271</v>
       </c>
       <c r="P90">
-        <f t="shared" si="12"/>
-        <v>158</v>
+        <f t="shared" si="11"/>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -15550,8 +15630,8 @@
         <v>284</v>
       </c>
       <c r="I91" s="4">
-        <f t="shared" si="11"/>
-        <v>171</v>
+        <f t="shared" si="12"/>
+        <v>182</v>
       </c>
       <c r="K91" s="1">
         <f t="shared" si="13"/>
@@ -15566,8 +15646,8 @@
         <v>280</v>
       </c>
       <c r="P91">
-        <f t="shared" si="12"/>
-        <v>171</v>
+        <f t="shared" si="11"/>
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -15601,8 +15681,8 @@
         <v>288</v>
       </c>
       <c r="I92" s="4">
-        <f t="shared" si="11"/>
-        <v>185</v>
+        <f t="shared" si="12"/>
+        <v>196</v>
       </c>
       <c r="K92" s="1">
         <f t="shared" si="13"/>
@@ -15617,8 +15697,8 @@
         <v>291</v>
       </c>
       <c r="P92">
-        <f t="shared" si="12"/>
-        <v>185</v>
+        <f t="shared" si="11"/>
+        <v>196</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -15652,8 +15732,8 @@
         <v>293</v>
       </c>
       <c r="I93" s="4">
-        <f t="shared" si="11"/>
-        <v>201</v>
+        <f t="shared" si="12"/>
+        <v>211</v>
       </c>
       <c r="K93" s="1">
         <f t="shared" si="13"/>
@@ -15668,8 +15748,8 @@
         <v>294</v>
       </c>
       <c r="P93">
-        <f t="shared" si="12"/>
-        <v>201</v>
+        <f t="shared" si="11"/>
+        <v>211</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -15703,8 +15783,8 @@
         <v>298</v>
       </c>
       <c r="I94" s="4">
-        <f t="shared" si="11"/>
-        <v>217</v>
+        <f t="shared" si="12"/>
+        <v>227</v>
       </c>
       <c r="K94" s="1">
         <f t="shared" si="13"/>
@@ -15719,8 +15799,8 @@
         <v>297</v>
       </c>
       <c r="P94">
-        <f t="shared" si="12"/>
-        <v>217</v>
+        <f t="shared" si="11"/>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -15754,8 +15834,8 @@
         <v>303</v>
       </c>
       <c r="I95" s="4">
-        <f t="shared" si="11"/>
-        <v>235</v>
+        <f t="shared" si="12"/>
+        <v>244</v>
       </c>
       <c r="K95" s="1">
         <f t="shared" si="13"/>
@@ -15770,8 +15850,8 @@
         <v>303</v>
       </c>
       <c r="P95">
-        <f t="shared" si="12"/>
-        <v>235</v>
+        <f t="shared" si="11"/>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -15805,8 +15885,8 @@
         <v>308</v>
       </c>
       <c r="I96" s="4">
-        <f t="shared" si="11"/>
-        <v>254</v>
+        <f t="shared" si="12"/>
+        <v>263</v>
       </c>
       <c r="K96" s="1">
         <f t="shared" si="13"/>
@@ -15821,8 +15901,8 @@
         <v>323</v>
       </c>
       <c r="P96">
-        <f t="shared" si="12"/>
-        <v>254</v>
+        <f t="shared" si="11"/>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -15856,8 +15936,8 @@
         <v>323</v>
       </c>
       <c r="I97" s="4">
-        <f t="shared" si="11"/>
-        <v>275</v>
+        <f t="shared" si="12"/>
+        <v>283</v>
       </c>
       <c r="K97" s="1">
         <f t="shared" si="13"/>
@@ -15872,8 +15952,8 @@
         <v>319</v>
       </c>
       <c r="P97">
-        <f t="shared" si="12"/>
-        <v>275</v>
+        <f t="shared" si="11"/>
+        <v>283</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -15907,8 +15987,8 @@
         <v>339</v>
       </c>
       <c r="I98" s="4">
-        <f t="shared" si="11"/>
-        <v>298</v>
+        <f t="shared" si="12"/>
+        <v>304</v>
       </c>
       <c r="K98" s="1">
         <f t="shared" si="13"/>
@@ -15923,8 +16003,8 @@
         <v>337</v>
       </c>
       <c r="P98">
-        <f t="shared" si="12"/>
-        <v>298</v>
+        <f t="shared" si="11"/>
+        <v>304</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
@@ -15958,8 +16038,8 @@
         <v>356</v>
       </c>
       <c r="I99" s="4">
-        <f t="shared" si="11"/>
-        <v>323</v>
+        <f t="shared" si="12"/>
+        <v>328</v>
       </c>
       <c r="K99" s="1">
         <f t="shared" si="13"/>
@@ -15974,8 +16054,8 @@
         <v>358</v>
       </c>
       <c r="P99">
-        <f t="shared" si="12"/>
-        <v>323</v>
+        <f t="shared" si="11"/>
+        <v>328</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -16009,8 +16089,8 @@
         <v>379</v>
       </c>
       <c r="I100" s="4">
-        <f t="shared" si="11"/>
-        <v>350</v>
+        <f t="shared" si="12"/>
+        <v>353</v>
       </c>
       <c r="K100" s="1">
         <f t="shared" si="13"/>
@@ -16025,8 +16105,8 @@
         <v>387</v>
       </c>
       <c r="P100">
-        <f t="shared" si="12"/>
-        <v>350</v>
+        <f t="shared" si="11"/>
+        <v>353</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -16060,8 +16140,8 @@
         <v>404</v>
       </c>
       <c r="I101" s="4">
-        <f t="shared" si="11"/>
-        <v>379</v>
+        <f t="shared" si="12"/>
+        <v>380</v>
       </c>
       <c r="K101" s="1">
         <f t="shared" si="13"/>
@@ -16076,8 +16156,8 @@
         <v>390</v>
       </c>
       <c r="P101">
-        <f t="shared" si="12"/>
-        <v>379</v>
+        <f t="shared" si="11"/>
+        <v>380</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
@@ -16111,8 +16191,8 @@
         <v>431</v>
       </c>
       <c r="I102" s="4">
-        <f t="shared" si="11"/>
-        <v>410</v>
+        <f t="shared" si="12"/>
+        <v>409</v>
       </c>
       <c r="K102" s="1">
         <f t="shared" si="13"/>
@@ -16127,8 +16207,8 @@
         <v>420</v>
       </c>
       <c r="P102">
-        <f t="shared" si="12"/>
-        <v>410</v>
+        <f t="shared" si="11"/>
+        <v>409</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -16162,8 +16242,8 @@
         <v>460</v>
       </c>
       <c r="I103" s="4">
-        <f t="shared" si="11"/>
-        <v>444</v>
+        <f t="shared" si="12"/>
+        <v>440</v>
       </c>
       <c r="K103" s="1">
         <f t="shared" si="13"/>
@@ -16178,8 +16258,8 @@
         <v>452</v>
       </c>
       <c r="P103">
-        <f t="shared" si="12"/>
-        <v>444</v>
+        <f t="shared" si="11"/>
+        <v>440</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -16213,8 +16293,8 @@
         <v>491</v>
       </c>
       <c r="I104" s="4">
-        <f t="shared" si="11"/>
-        <v>481</v>
+        <f t="shared" si="12"/>
+        <v>473</v>
       </c>
       <c r="K104" s="1">
         <f t="shared" si="13"/>
@@ -16229,8 +16309,8 @@
         <v>514</v>
       </c>
       <c r="P104">
-        <f t="shared" si="12"/>
-        <v>481</v>
+        <f t="shared" si="11"/>
+        <v>473</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -16241,15 +16321,15 @@
         <v>100</v>
       </c>
       <c r="C105">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D105">
         <f t="shared" si="15"/>
-        <v>29998302</v>
+        <v>29998303</v>
       </c>
       <c r="E105">
         <f t="shared" si="16"/>
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F105">
         <f t="shared" si="17"/>
@@ -16257,15 +16337,15 @@
       </c>
       <c r="G105" s="2">
         <f t="shared" si="18"/>
-        <v>29998302</v>
+        <v>29998303</v>
       </c>
       <c r="H105" s="2">
         <f t="shared" si="19"/>
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I105" s="4">
-        <f t="shared" si="11"/>
-        <v>521</v>
+        <f t="shared" si="12"/>
+        <v>510</v>
       </c>
       <c r="K105" s="1">
         <f t="shared" si="13"/>
@@ -16273,15 +16353,15 @@
       </c>
       <c r="L105">
         <f t="shared" si="14"/>
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="M105">
         <f>RealData!B102</f>
         <v>539</v>
       </c>
       <c r="P105">
-        <f t="shared" si="12"/>
-        <v>521</v>
+        <f t="shared" si="11"/>
+        <v>510</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -16292,15 +16372,15 @@
         <v>101</v>
       </c>
       <c r="C106">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D106">
         <f t="shared" si="15"/>
-        <v>29998216</v>
+        <v>29998218</v>
       </c>
       <c r="E106">
         <f t="shared" si="16"/>
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F106">
         <f t="shared" si="17"/>
@@ -16308,15 +16388,15 @@
       </c>
       <c r="G106" s="2">
         <f t="shared" si="18"/>
-        <v>29998216</v>
+        <v>29998218</v>
       </c>
       <c r="H106" s="2">
         <f t="shared" si="19"/>
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I106" s="4">
-        <f t="shared" si="11"/>
-        <v>565</v>
+        <f t="shared" si="12"/>
+        <v>549</v>
       </c>
       <c r="K106" s="1">
         <f t="shared" si="13"/>
@@ -16324,15 +16404,15 @@
       </c>
       <c r="L106">
         <f t="shared" si="14"/>
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="M106">
         <f>RealData!B103</f>
         <v>586</v>
       </c>
       <c r="P106">
-        <f t="shared" si="12"/>
-        <v>565</v>
+        <f t="shared" si="11"/>
+        <v>549</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
@@ -16343,15 +16423,15 @@
         <v>102</v>
       </c>
       <c r="C107">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D107">
         <f t="shared" si="15"/>
-        <v>29998123</v>
+        <v>29998127</v>
       </c>
       <c r="E107">
         <f t="shared" si="16"/>
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="F107">
         <f t="shared" si="17"/>
@@ -16359,15 +16439,15 @@
       </c>
       <c r="G107" s="2">
         <f t="shared" si="18"/>
-        <v>29998123</v>
+        <v>29998127</v>
       </c>
       <c r="H107" s="2">
         <f t="shared" si="19"/>
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="I107" s="4">
-        <f t="shared" si="11"/>
-        <v>612</v>
+        <f t="shared" si="12"/>
+        <v>591</v>
       </c>
       <c r="K107" s="1">
         <f t="shared" si="13"/>
@@ -16375,15 +16455,15 @@
       </c>
       <c r="L107">
         <f t="shared" si="14"/>
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="M107">
         <f>RealData!B104</f>
         <v>638</v>
       </c>
       <c r="P107">
-        <f t="shared" si="12"/>
-        <v>612</v>
+        <f t="shared" si="11"/>
+        <v>591</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
@@ -16394,15 +16474,15 @@
         <v>103</v>
       </c>
       <c r="C108">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D108">
         <f t="shared" si="15"/>
-        <v>29998023</v>
+        <v>29998029</v>
       </c>
       <c r="E108">
         <f t="shared" si="16"/>
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="F108">
         <f t="shared" si="17"/>
@@ -16410,15 +16490,15 @@
       </c>
       <c r="G108" s="2">
         <f t="shared" si="18"/>
-        <v>29998023</v>
+        <v>29998029</v>
       </c>
       <c r="H108" s="2">
         <f t="shared" si="19"/>
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="I108" s="4">
-        <f t="shared" si="11"/>
-        <v>663</v>
+        <f t="shared" si="12"/>
+        <v>637</v>
       </c>
       <c r="K108" s="1">
         <f t="shared" si="13"/>
@@ -16426,15 +16506,15 @@
       </c>
       <c r="L108">
         <f t="shared" si="14"/>
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="M108">
         <f>RealData!B105</f>
         <v>705</v>
       </c>
       <c r="P108">
-        <f t="shared" si="12"/>
-        <v>663</v>
+        <f t="shared" si="11"/>
+        <v>637</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -16445,31 +16525,31 @@
         <v>104</v>
       </c>
       <c r="C109">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D109">
         <f t="shared" si="15"/>
-        <v>29997915</v>
+        <v>29997923</v>
       </c>
       <c r="E109">
         <f t="shared" si="16"/>
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="F109">
         <f t="shared" si="17"/>
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="G109" s="2">
         <f t="shared" si="18"/>
-        <v>29997915</v>
+        <v>29997923</v>
       </c>
       <c r="H109" s="2">
         <f t="shared" si="19"/>
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="I109" s="4">
-        <f t="shared" si="11"/>
-        <v>718</v>
+        <f t="shared" si="12"/>
+        <v>686</v>
       </c>
       <c r="K109" s="1">
         <f t="shared" si="13"/>
@@ -16477,15 +16557,15 @@
       </c>
       <c r="L109">
         <f t="shared" si="14"/>
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="M109">
         <f>RealData!B106</f>
         <v>750</v>
       </c>
       <c r="P109">
-        <f t="shared" si="12"/>
-        <v>718</v>
+        <f t="shared" si="11"/>
+        <v>686</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -16496,31 +16576,31 @@
         <v>105</v>
       </c>
       <c r="C110">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D110">
         <f t="shared" si="15"/>
-        <v>29997798</v>
+        <v>29997809</v>
       </c>
       <c r="E110">
         <f t="shared" si="16"/>
-        <v>775</v>
+        <v>766</v>
       </c>
       <c r="F110">
         <f t="shared" si="17"/>
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="G110" s="2">
         <f t="shared" si="18"/>
-        <v>29997798</v>
+        <v>29997809</v>
       </c>
       <c r="H110" s="2">
         <f t="shared" si="19"/>
-        <v>775</v>
+        <v>766</v>
       </c>
       <c r="I110" s="4">
-        <f t="shared" si="11"/>
-        <v>778</v>
+        <f t="shared" si="12"/>
+        <v>739</v>
       </c>
       <c r="K110" s="1">
         <f t="shared" si="13"/>
@@ -16528,15 +16608,15 @@
       </c>
       <c r="L110">
         <f t="shared" si="14"/>
-        <v>775</v>
+        <v>766</v>
       </c>
       <c r="M110">
         <f>RealData!B107</f>
         <v>797</v>
       </c>
       <c r="P110">
-        <f t="shared" si="12"/>
-        <v>778</v>
+        <f t="shared" si="11"/>
+        <v>739</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
@@ -16547,31 +16627,31 @@
         <v>106</v>
       </c>
       <c r="C111">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D111">
         <f t="shared" si="15"/>
-        <v>29997672</v>
+        <v>29997686</v>
       </c>
       <c r="E111">
         <f t="shared" si="16"/>
-        <v>836</v>
+        <v>825</v>
       </c>
       <c r="F111">
         <f t="shared" si="17"/>
-        <v>1492</v>
+        <v>1489</v>
       </c>
       <c r="G111" s="2">
         <f t="shared" si="18"/>
-        <v>29997672</v>
+        <v>29997686</v>
       </c>
       <c r="H111" s="2">
         <f t="shared" si="19"/>
-        <v>836</v>
+        <v>825</v>
       </c>
       <c r="I111" s="4">
-        <f t="shared" si="11"/>
-        <v>843</v>
+        <f t="shared" si="12"/>
+        <v>795</v>
       </c>
       <c r="K111" s="1">
         <f t="shared" si="13"/>
@@ -16579,15 +16659,15 @@
       </c>
       <c r="L111">
         <f t="shared" si="14"/>
-        <v>836</v>
+        <v>825</v>
       </c>
       <c r="M111">
         <f>RealData!B108</f>
         <v>870</v>
       </c>
       <c r="P111">
-        <f t="shared" si="12"/>
-        <v>843</v>
+        <f t="shared" si="11"/>
+        <v>795</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -16598,31 +16678,31 @@
         <v>107</v>
       </c>
       <c r="C112">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D112">
         <f t="shared" si="15"/>
-        <v>29997536</v>
+        <v>29997554</v>
       </c>
       <c r="E112">
         <f t="shared" si="16"/>
-        <v>902</v>
+        <v>888</v>
       </c>
       <c r="F112">
         <f t="shared" si="17"/>
-        <v>1562</v>
+        <v>1558</v>
       </c>
       <c r="G112" s="2">
         <f t="shared" si="18"/>
-        <v>29997536</v>
+        <v>29997554</v>
       </c>
       <c r="H112" s="2">
         <f t="shared" si="19"/>
-        <v>902</v>
+        <v>888</v>
       </c>
       <c r="I112" s="4">
         <f t="shared" ref="I112:I113" si="20">I111+ROUND(($D$1/$D$2)*G111*(I111/$D$3),0)-ROUND(I111/$D$2,0)</f>
-        <v>913</v>
+        <v>856</v>
       </c>
       <c r="K112" s="1">
         <f t="shared" si="13"/>
@@ -16630,15 +16710,15 @@
       </c>
       <c r="L112">
         <f t="shared" si="14"/>
-        <v>902</v>
+        <v>888</v>
       </c>
       <c r="M112">
         <f>RealData!B109</f>
         <v>926</v>
       </c>
       <c r="P112">
-        <f t="shared" si="12"/>
-        <v>913</v>
+        <f t="shared" si="11"/>
+        <v>856</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
@@ -16649,31 +16729,31 @@
         <v>108</v>
       </c>
       <c r="C113">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="D113">
         <f t="shared" si="15"/>
-        <v>29997389</v>
+        <v>29997412</v>
       </c>
       <c r="E113">
         <f t="shared" si="16"/>
-        <v>974</v>
+        <v>956</v>
       </c>
       <c r="F113">
         <f t="shared" si="17"/>
-        <v>1637</v>
+        <v>1632</v>
       </c>
       <c r="G113" s="2">
         <f t="shared" si="18"/>
-        <v>29997389</v>
+        <v>29997412</v>
       </c>
       <c r="H113" s="2">
-        <f t="shared" si="19"/>
-        <v>974</v>
+        <f>E113</f>
+        <v>956</v>
       </c>
       <c r="I113" s="4">
         <f t="shared" si="20"/>
-        <v>989</v>
+        <v>922</v>
       </c>
       <c r="K113" s="1">
         <f t="shared" si="13"/>
@@ -16681,7 +16761,7 @@
       </c>
       <c r="L113">
         <f t="shared" si="14"/>
-        <v>974</v>
+        <v>956</v>
       </c>
       <c r="M113">
         <f>RealData!B110</f>
@@ -16689,15 +16769,15 @@
       </c>
       <c r="N113">
         <f>E113</f>
-        <v>974</v>
+        <v>956</v>
       </c>
       <c r="O113">
         <f>H113</f>
-        <v>974</v>
+        <v>956</v>
       </c>
       <c r="P113">
-        <f t="shared" si="12"/>
-        <v>989</v>
+        <f>I113</f>
+        <v>922</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
@@ -16707,32 +16787,32 @@
       <c r="B114" s="4">
         <v>109</v>
       </c>
-      <c r="C114">
-        <v>1.95</v>
+      <c r="C114" s="4">
+        <v>1.92</v>
       </c>
       <c r="D114" s="4">
         <f t="shared" si="15"/>
-        <v>29997231</v>
+        <v>29997259</v>
       </c>
       <c r="E114" s="4">
         <f t="shared" si="16"/>
-        <v>1051</v>
+        <v>1029</v>
       </c>
       <c r="F114" s="4">
         <f t="shared" si="17"/>
-        <v>1718</v>
+        <v>1712</v>
       </c>
       <c r="G114" s="4">
         <f t="shared" si="18"/>
-        <v>29997231</v>
+        <v>29997259</v>
       </c>
       <c r="H114" s="4">
         <f>H113+ROUND(($D$1/$D$2)*G113*(H113/$D$3),0)-ROUND(H113/$D$2,0)</f>
-        <v>1055</v>
+        <v>1029</v>
       </c>
       <c r="I114" s="4">
         <f>I113+ROUND(($D$1/$D$2)*G113*(I113/$D$3),0)-ROUND(I113/$D$2,0)</f>
-        <v>1072</v>
+        <v>993</v>
       </c>
       <c r="K114" s="1">
         <f t="shared" si="13"/>
@@ -16740,7 +16820,7 @@
       </c>
       <c r="L114">
         <f t="shared" ref="L114" si="21">E114</f>
-        <v>1051</v>
+        <v>1029</v>
       </c>
       <c r="M114">
         <f>RealData!B111</f>
@@ -16748,15 +16828,15 @@
       </c>
       <c r="N114">
         <f>E114</f>
-        <v>1051</v>
+        <v>1029</v>
       </c>
       <c r="O114">
         <f>H114</f>
-        <v>1055</v>
+        <v>1029</v>
       </c>
       <c r="P114">
-        <f t="shared" si="12"/>
-        <v>1072</v>
+        <f t="shared" si="11"/>
+        <v>993</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
@@ -16766,48 +16846,56 @@
       <c r="B115" s="4">
         <v>110</v>
       </c>
-      <c r="C115">
-        <v>1.95</v>
+      <c r="C115" s="4">
+        <v>1.92</v>
       </c>
       <c r="D115" s="4">
         <f t="shared" si="15"/>
-        <v>29997060</v>
+        <v>29997094</v>
       </c>
       <c r="E115" s="4">
         <f t="shared" si="16"/>
-        <v>1134</v>
+        <v>1108</v>
       </c>
       <c r="F115" s="4">
         <f t="shared" si="17"/>
-        <v>1806</v>
+        <v>1798</v>
       </c>
       <c r="G115" s="4">
         <f t="shared" si="18"/>
-        <v>29997060</v>
+        <v>29997094</v>
       </c>
       <c r="H115" s="4">
         <f t="shared" ref="H115:H122" si="22">H114+ROUND(($D$1/$D$2)*G114*(H114/$D$3),0)-ROUND(H114/$D$2,0)</f>
-        <v>1143</v>
+        <v>1108</v>
       </c>
       <c r="I115" s="4">
         <f t="shared" ref="I115:I134" si="23">I114+ROUND(($D$1/$D$2)*G114*(I114/$D$3),0)-ROUND(I114/$D$2,0)</f>
-        <v>1162</v>
+        <v>1069</v>
       </c>
       <c r="K115" s="1">
         <f t="shared" si="13"/>
         <v>44128</v>
       </c>
+      <c r="L115">
+        <f>E115</f>
+        <v>1108</v>
+      </c>
+      <c r="M115">
+        <f>RealData!B112</f>
+        <v>1128</v>
+      </c>
       <c r="N115">
         <f t="shared" ref="N115:N134" si="24">E115</f>
-        <v>1134</v>
+        <v>1108</v>
       </c>
       <c r="O115">
         <f t="shared" ref="O115:O134" si="25">H115</f>
-        <v>1143</v>
+        <v>1108</v>
       </c>
       <c r="P115">
-        <f t="shared" si="12"/>
-        <v>1162</v>
+        <f t="shared" si="11"/>
+        <v>1069</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
@@ -16817,48 +16905,56 @@
       <c r="B116" s="4">
         <v>111</v>
       </c>
-      <c r="C116">
-        <v>1.95</v>
+      <c r="C116" s="4">
+        <v>1.92</v>
       </c>
       <c r="D116" s="4">
         <f t="shared" si="15"/>
-        <v>29996876</v>
+        <v>29996917</v>
       </c>
       <c r="E116" s="4">
         <f t="shared" si="16"/>
-        <v>1223</v>
+        <v>1193</v>
       </c>
       <c r="F116" s="4">
         <f t="shared" si="17"/>
-        <v>1901</v>
+        <v>1890</v>
       </c>
       <c r="G116" s="4">
         <f t="shared" si="18"/>
-        <v>29996876</v>
+        <v>29996917</v>
       </c>
       <c r="H116" s="4">
         <f t="shared" si="22"/>
-        <v>1238</v>
+        <v>1193</v>
       </c>
       <c r="I116" s="4">
         <f t="shared" si="23"/>
-        <v>1259</v>
+        <v>1151</v>
       </c>
       <c r="K116" s="1">
         <f t="shared" si="13"/>
         <v>44129</v>
       </c>
+      <c r="L116">
+        <f t="shared" ref="L116:L117" si="26">E116</f>
+        <v>1193</v>
+      </c>
+      <c r="M116">
+        <f>RealData!B113</f>
+        <v>1208</v>
+      </c>
       <c r="N116">
         <f t="shared" si="24"/>
-        <v>1223</v>
+        <v>1193</v>
       </c>
       <c r="O116">
         <f t="shared" si="25"/>
-        <v>1238</v>
+        <v>1193</v>
       </c>
       <c r="P116">
-        <f t="shared" si="12"/>
-        <v>1259</v>
+        <f t="shared" si="11"/>
+        <v>1151</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -16868,48 +16964,56 @@
       <c r="B117" s="4">
         <v>112</v>
       </c>
-      <c r="C117">
-        <v>1.95</v>
+      <c r="C117" s="4">
+        <v>1.92</v>
       </c>
       <c r="D117" s="4">
         <f t="shared" si="15"/>
-        <v>29996677</v>
+        <v>29996726</v>
       </c>
       <c r="E117" s="4">
         <f t="shared" si="16"/>
-        <v>1320</v>
+        <v>1285</v>
       </c>
       <c r="F117" s="4">
         <f t="shared" si="17"/>
-        <v>2003</v>
+        <v>1989</v>
       </c>
       <c r="G117" s="4">
         <f t="shared" si="18"/>
-        <v>29996677</v>
+        <v>29996726</v>
       </c>
       <c r="H117" s="4">
         <f t="shared" si="22"/>
-        <v>1341</v>
+        <v>1285</v>
       </c>
       <c r="I117" s="4">
         <f t="shared" si="23"/>
-        <v>1364</v>
+        <v>1239</v>
       </c>
       <c r="K117" s="1">
         <f t="shared" si="13"/>
         <v>44130</v>
       </c>
+      <c r="L117">
+        <f t="shared" si="26"/>
+        <v>1285</v>
+      </c>
+      <c r="M117">
+        <f>RealData!B114</f>
+        <v>1284</v>
+      </c>
       <c r="N117">
         <f t="shared" si="24"/>
-        <v>1320</v>
+        <v>1285</v>
       </c>
       <c r="O117">
         <f t="shared" si="25"/>
-        <v>1341</v>
+        <v>1285</v>
       </c>
       <c r="P117">
-        <f t="shared" si="12"/>
-        <v>1364</v>
+        <f t="shared" si="11"/>
+        <v>1239</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
@@ -16919,32 +17023,32 @@
       <c r="B118" s="4">
         <v>113</v>
       </c>
-      <c r="C118">
-        <v>1.95</v>
+      <c r="C118" s="4">
+        <v>1.92</v>
       </c>
       <c r="D118" s="4">
         <f t="shared" si="15"/>
-        <v>29996463</v>
+        <v>29996520</v>
       </c>
       <c r="E118" s="4">
         <f t="shared" si="16"/>
-        <v>1424</v>
+        <v>1384</v>
       </c>
       <c r="F118" s="4">
         <f t="shared" si="17"/>
-        <v>2113</v>
+        <v>2096</v>
       </c>
       <c r="G118" s="4">
         <f t="shared" si="18"/>
-        <v>29996463</v>
+        <v>29996520</v>
       </c>
       <c r="H118" s="4">
         <f t="shared" si="22"/>
-        <v>1452</v>
+        <v>1384</v>
       </c>
       <c r="I118" s="4">
         <f t="shared" si="23"/>
-        <v>1477</v>
+        <v>1334</v>
       </c>
       <c r="K118" s="1">
         <f t="shared" si="13"/>
@@ -16952,15 +17056,15 @@
       </c>
       <c r="N118">
         <f t="shared" si="24"/>
-        <v>1424</v>
+        <v>1384</v>
       </c>
       <c r="O118">
         <f t="shared" si="25"/>
-        <v>1452</v>
+        <v>1384</v>
       </c>
       <c r="P118">
-        <f t="shared" si="12"/>
-        <v>1477</v>
+        <f t="shared" si="11"/>
+        <v>1334</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
@@ -16970,32 +17074,32 @@
       <c r="B119" s="4">
         <v>114</v>
       </c>
-      <c r="C119">
-        <v>1.95</v>
+      <c r="C119" s="4">
+        <v>1.92</v>
       </c>
       <c r="D119" s="4">
         <f t="shared" si="15"/>
-        <v>29996232</v>
+        <v>29996299</v>
       </c>
       <c r="E119" s="4">
         <f t="shared" si="16"/>
-        <v>1536</v>
+        <v>1490</v>
       </c>
       <c r="F119" s="4">
         <f t="shared" si="17"/>
-        <v>2232</v>
+        <v>2211</v>
       </c>
       <c r="G119" s="4">
         <f t="shared" si="18"/>
-        <v>29996232</v>
+        <v>29996299</v>
       </c>
       <c r="H119" s="4">
         <f t="shared" si="22"/>
-        <v>1573</v>
+        <v>1490</v>
       </c>
       <c r="I119" s="4">
         <f t="shared" si="23"/>
-        <v>1600</v>
+        <v>1436</v>
       </c>
       <c r="K119" s="1">
         <f t="shared" si="13"/>
@@ -17003,15 +17107,15 @@
       </c>
       <c r="N119">
         <f t="shared" si="24"/>
-        <v>1536</v>
+        <v>1490</v>
       </c>
       <c r="O119">
         <f t="shared" si="25"/>
-        <v>1573</v>
+        <v>1490</v>
       </c>
       <c r="P119">
-        <f t="shared" ref="P119:P134" si="26">I119</f>
-        <v>1600</v>
+        <f t="shared" ref="P119:P134" si="27">I119</f>
+        <v>1436</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
@@ -17021,32 +17125,32 @@
       <c r="B120" s="4">
         <v>115</v>
       </c>
-      <c r="C120">
-        <v>1.95</v>
+      <c r="C120" s="4">
+        <v>1.92</v>
       </c>
       <c r="D120" s="4">
         <f t="shared" si="15"/>
-        <v>29995982</v>
+        <v>29996061</v>
       </c>
       <c r="E120" s="4">
         <f t="shared" si="16"/>
-        <v>1658</v>
+        <v>1604</v>
       </c>
       <c r="F120" s="4">
         <f t="shared" si="17"/>
-        <v>2360</v>
+        <v>2335</v>
       </c>
       <c r="G120" s="4">
         <f t="shared" si="18"/>
-        <v>29995982</v>
+        <v>29996061</v>
       </c>
       <c r="H120" s="4">
         <f t="shared" si="22"/>
-        <v>1704</v>
+        <v>1604</v>
       </c>
       <c r="I120" s="4">
         <f t="shared" si="23"/>
-        <v>1734</v>
+        <v>1546</v>
       </c>
       <c r="K120" s="1">
         <f t="shared" si="13"/>
@@ -17054,15 +17158,15 @@
       </c>
       <c r="N120">
         <f t="shared" si="24"/>
-        <v>1658</v>
+        <v>1604</v>
       </c>
       <c r="O120">
         <f t="shared" si="25"/>
-        <v>1704</v>
+        <v>1604</v>
       </c>
       <c r="P120">
-        <f t="shared" si="26"/>
-        <v>1734</v>
+        <f t="shared" si="27"/>
+        <v>1546</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
@@ -17077,27 +17181,27 @@
       </c>
       <c r="D121" s="6">
         <f t="shared" si="15"/>
-        <v>29995733</v>
+        <v>29995820</v>
       </c>
       <c r="E121" s="6">
         <f t="shared" si="16"/>
-        <v>1769</v>
+        <v>1711</v>
       </c>
       <c r="F121" s="6">
         <f t="shared" si="17"/>
-        <v>2498</v>
+        <v>2469</v>
       </c>
       <c r="G121" s="6">
         <f t="shared" si="18"/>
-        <v>29995733</v>
+        <v>29995820</v>
       </c>
       <c r="H121" s="6">
         <f t="shared" si="22"/>
-        <v>1846</v>
+        <v>1727</v>
       </c>
       <c r="I121" s="4">
         <f t="shared" si="23"/>
-        <v>1878</v>
+        <v>1664</v>
       </c>
       <c r="K121" s="1">
         <f t="shared" si="13"/>
@@ -17105,15 +17209,15 @@
       </c>
       <c r="N121">
         <f t="shared" si="24"/>
-        <v>1769</v>
+        <v>1711</v>
       </c>
       <c r="O121">
         <f t="shared" si="25"/>
-        <v>1846</v>
+        <v>1727</v>
       </c>
       <c r="P121">
-        <f t="shared" si="26"/>
-        <v>1878</v>
+        <f t="shared" si="27"/>
+        <v>1664</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
@@ -17128,27 +17232,27 @@
       </c>
       <c r="D122" s="6">
         <f t="shared" si="15"/>
-        <v>29995468</v>
+        <v>29995563</v>
       </c>
       <c r="E122" s="6">
         <f t="shared" si="16"/>
-        <v>1887</v>
+        <v>1825</v>
       </c>
       <c r="F122" s="6">
         <f t="shared" si="17"/>
-        <v>2645</v>
+        <v>2612</v>
       </c>
       <c r="G122" s="6">
         <f t="shared" si="18"/>
-        <v>29995468</v>
+        <v>29995563</v>
       </c>
       <c r="H122" s="6">
         <f t="shared" si="22"/>
-        <v>2000</v>
+        <v>1859</v>
       </c>
       <c r="I122" s="4">
         <f t="shared" si="23"/>
-        <v>2034</v>
+        <v>1791</v>
       </c>
       <c r="K122" s="1">
         <f t="shared" si="13"/>
@@ -17156,15 +17260,15 @@
       </c>
       <c r="N122">
         <f t="shared" si="24"/>
-        <v>1887</v>
+        <v>1825</v>
       </c>
       <c r="O122">
         <f t="shared" si="25"/>
-        <v>2000</v>
+        <v>1859</v>
       </c>
       <c r="P122">
-        <f t="shared" si="26"/>
-        <v>2034</v>
+        <f t="shared" si="27"/>
+        <v>1791</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
@@ -17178,28 +17282,28 @@
         <v>1.8</v>
       </c>
       <c r="D123" s="6">
-        <f t="shared" ref="D123:D132" si="27">D122-ROUND((C123/$D$2)*D122*(E122/$D$3),0)</f>
-        <v>29995185</v>
+        <f t="shared" ref="D123:D132" si="28">D122-ROUND((C123/$D$2)*D122*(E122/$D$3),0)</f>
+        <v>29995289</v>
       </c>
       <c r="E123" s="6">
-        <f t="shared" ref="E123:E132" si="28">E122+ROUND((C123/$D$2)*D122*(E122/$D$3),0)-ROUND(E122/$D$2,0)</f>
-        <v>2013</v>
+        <f t="shared" ref="E123:E132" si="29">E122+ROUND((C123/$D$2)*D122*(E122/$D$3),0)-ROUND(E122/$D$2,0)</f>
+        <v>1947</v>
       </c>
       <c r="F123" s="6">
-        <f t="shared" ref="F123:F132" si="29">F122+ROUND(E122/$D$2,0)</f>
-        <v>2802</v>
+        <f t="shared" ref="F123:F132" si="30">F122+ROUND(E122/$D$2,0)</f>
+        <v>2764</v>
       </c>
       <c r="G123" s="6">
-        <f t="shared" ref="G123:G132" si="30">D123</f>
-        <v>29995185</v>
+        <f t="shared" ref="G123:G132" si="31">D123</f>
+        <v>29995289</v>
       </c>
       <c r="H123" s="6">
-        <f t="shared" ref="H123:H132" si="31">H122+ROUND(($D$1/$D$2)*G122*(H122/$D$3),0)-ROUND(H122/$D$2,0)</f>
-        <v>2166</v>
+        <f t="shared" ref="H123:H132" si="32">H122+ROUND(($D$1/$D$2)*G122*(H122/$D$3),0)-ROUND(H122/$D$2,0)</f>
+        <v>2001</v>
       </c>
       <c r="I123" s="4">
         <f t="shared" si="23"/>
-        <v>2203</v>
+        <v>1929</v>
       </c>
       <c r="K123" s="1">
         <f t="shared" si="13"/>
@@ -17207,15 +17311,15 @@
       </c>
       <c r="N123">
         <f t="shared" si="24"/>
-        <v>2013</v>
+        <v>1947</v>
       </c>
       <c r="O123">
         <f t="shared" si="25"/>
-        <v>2166</v>
+        <v>2001</v>
       </c>
       <c r="P123">
-        <f t="shared" si="26"/>
-        <v>2203</v>
+        <f t="shared" si="27"/>
+        <v>1929</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
@@ -17229,28 +17333,28 @@
         <v>1.8</v>
       </c>
       <c r="D124" s="6">
-        <f t="shared" si="27"/>
-        <v>29994883</v>
+        <f t="shared" si="28"/>
+        <v>29994997</v>
       </c>
       <c r="E124" s="6">
-        <f t="shared" si="28"/>
-        <v>2147</v>
+        <f t="shared" si="29"/>
+        <v>2077</v>
       </c>
       <c r="F124" s="6">
-        <f t="shared" si="29"/>
-        <v>2970</v>
+        <f t="shared" si="30"/>
+        <v>2926</v>
       </c>
       <c r="G124" s="6">
-        <f t="shared" si="30"/>
-        <v>29994883</v>
+        <f t="shared" si="31"/>
+        <v>29994997</v>
       </c>
       <c r="H124" s="6">
-        <f t="shared" si="31"/>
-        <v>2346</v>
+        <f t="shared" si="32"/>
+        <v>2154</v>
       </c>
       <c r="I124" s="4">
         <f t="shared" si="23"/>
-        <v>2386</v>
+        <v>2077</v>
       </c>
       <c r="K124" s="1">
         <f t="shared" si="13"/>
@@ -17258,15 +17362,15 @@
       </c>
       <c r="N124">
         <f t="shared" si="24"/>
-        <v>2147</v>
+        <v>2077</v>
       </c>
       <c r="O124">
         <f t="shared" si="25"/>
-        <v>2346</v>
+        <v>2154</v>
       </c>
       <c r="P124">
-        <f t="shared" si="26"/>
-        <v>2386</v>
+        <f t="shared" si="27"/>
+        <v>2077</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -17280,28 +17384,28 @@
         <v>1.8</v>
       </c>
       <c r="D125" s="6">
-        <f t="shared" si="27"/>
-        <v>29994561</v>
+        <f t="shared" si="28"/>
+        <v>29994686</v>
       </c>
       <c r="E125" s="6">
-        <f t="shared" si="28"/>
-        <v>2290</v>
+        <f t="shared" si="29"/>
+        <v>2215</v>
       </c>
       <c r="F125" s="6">
-        <f t="shared" si="29"/>
-        <v>3149</v>
+        <f t="shared" si="30"/>
+        <v>3099</v>
       </c>
       <c r="G125" s="6">
-        <f t="shared" si="30"/>
-        <v>29994561</v>
+        <f t="shared" si="31"/>
+        <v>29994686</v>
       </c>
       <c r="H125" s="6">
-        <f t="shared" si="31"/>
-        <v>2541</v>
+        <f t="shared" si="32"/>
+        <v>2319</v>
       </c>
       <c r="I125" s="4">
         <f t="shared" si="23"/>
-        <v>2585</v>
+        <v>2236</v>
       </c>
       <c r="K125" s="1">
         <f t="shared" si="13"/>
@@ -17309,15 +17413,15 @@
       </c>
       <c r="N125">
         <f t="shared" si="24"/>
-        <v>2290</v>
+        <v>2215</v>
       </c>
       <c r="O125">
         <f t="shared" si="25"/>
-        <v>2541</v>
+        <v>2319</v>
       </c>
       <c r="P125">
-        <f t="shared" si="26"/>
-        <v>2585</v>
+        <f t="shared" si="27"/>
+        <v>2236</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
@@ -17331,28 +17435,28 @@
         <v>1.8</v>
       </c>
       <c r="D126" s="6">
-        <f t="shared" si="27"/>
-        <v>29994218</v>
+        <f t="shared" si="28"/>
+        <v>29994354</v>
       </c>
       <c r="E126" s="6">
-        <f t="shared" si="28"/>
-        <v>2442</v>
+        <f t="shared" si="29"/>
+        <v>2362</v>
       </c>
       <c r="F126" s="6">
-        <f t="shared" si="29"/>
-        <v>3340</v>
+        <f t="shared" si="30"/>
+        <v>3284</v>
       </c>
       <c r="G126" s="6">
-        <f t="shared" si="30"/>
-        <v>29994218</v>
+        <f t="shared" si="31"/>
+        <v>29994354</v>
       </c>
       <c r="H126" s="6">
-        <f t="shared" si="31"/>
-        <v>2752</v>
+        <f t="shared" si="32"/>
+        <v>2497</v>
       </c>
       <c r="I126" s="4">
         <f t="shared" si="23"/>
-        <v>2801</v>
+        <v>2408</v>
       </c>
       <c r="K126" s="1">
         <f t="shared" si="13"/>
@@ -17360,15 +17464,15 @@
       </c>
       <c r="N126">
         <f t="shared" si="24"/>
-        <v>2442</v>
+        <v>2362</v>
       </c>
       <c r="O126">
         <f t="shared" si="25"/>
-        <v>2752</v>
+        <v>2497</v>
       </c>
       <c r="P126">
-        <f t="shared" si="26"/>
-        <v>2801</v>
+        <f t="shared" si="27"/>
+        <v>2408</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
@@ -17382,28 +17486,28 @@
         <v>1.8</v>
       </c>
       <c r="D127" s="6">
-        <f t="shared" si="27"/>
-        <v>29993852</v>
+        <f t="shared" si="28"/>
+        <v>29994000</v>
       </c>
       <c r="E127" s="6">
-        <f t="shared" si="28"/>
-        <v>2604</v>
+        <f t="shared" si="29"/>
+        <v>2519</v>
       </c>
       <c r="F127" s="6">
-        <f t="shared" si="29"/>
-        <v>3544</v>
+        <f t="shared" si="30"/>
+        <v>3481</v>
       </c>
       <c r="G127" s="6">
-        <f t="shared" si="30"/>
-        <v>29993852</v>
+        <f t="shared" si="31"/>
+        <v>29994000</v>
       </c>
       <c r="H127" s="6">
-        <f t="shared" si="31"/>
-        <v>2982</v>
+        <f t="shared" si="32"/>
+        <v>2688</v>
       </c>
       <c r="I127" s="4">
         <f t="shared" si="23"/>
-        <v>3035</v>
+        <v>2592</v>
       </c>
       <c r="K127" s="1">
         <f t="shared" si="13"/>
@@ -17411,15 +17515,15 @@
       </c>
       <c r="N127">
         <f t="shared" si="24"/>
-        <v>2604</v>
+        <v>2519</v>
       </c>
       <c r="O127">
         <f t="shared" si="25"/>
-        <v>2982</v>
+        <v>2688</v>
       </c>
       <c r="P127">
-        <f t="shared" si="26"/>
-        <v>3035</v>
+        <f t="shared" si="27"/>
+        <v>2592</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
@@ -17433,28 +17537,28 @@
         <v>1.6</v>
       </c>
       <c r="D128">
-        <f t="shared" si="27"/>
-        <v>29993505</v>
+        <f t="shared" si="28"/>
+        <v>29993664</v>
       </c>
       <c r="E128">
-        <f t="shared" si="28"/>
-        <v>2734</v>
+        <f t="shared" si="29"/>
+        <v>2645</v>
       </c>
       <c r="F128">
-        <f t="shared" si="29"/>
-        <v>3761</v>
+        <f t="shared" si="30"/>
+        <v>3691</v>
       </c>
       <c r="G128" s="2">
-        <f t="shared" si="30"/>
-        <v>29993505</v>
+        <f t="shared" si="31"/>
+        <v>29993664</v>
       </c>
       <c r="H128">
-        <f t="shared" si="31"/>
-        <v>3230</v>
+        <f t="shared" si="32"/>
+        <v>2894</v>
       </c>
       <c r="I128" s="4">
         <f t="shared" si="23"/>
-        <v>3288</v>
+        <v>2791</v>
       </c>
       <c r="K128" s="1">
         <f t="shared" si="13"/>
@@ -17462,15 +17566,15 @@
       </c>
       <c r="N128">
         <f t="shared" si="24"/>
-        <v>2734</v>
+        <v>2645</v>
       </c>
       <c r="O128">
         <f t="shared" si="25"/>
-        <v>3230</v>
+        <v>2894</v>
       </c>
       <c r="P128">
-        <f t="shared" si="26"/>
-        <v>3288</v>
+        <f t="shared" si="27"/>
+        <v>2791</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
@@ -17484,28 +17588,28 @@
         <v>1.6</v>
       </c>
       <c r="D129">
-        <f t="shared" si="27"/>
-        <v>29993141</v>
+        <f t="shared" si="28"/>
+        <v>29993311</v>
       </c>
       <c r="E129">
-        <f t="shared" si="28"/>
-        <v>2870</v>
+        <f t="shared" si="29"/>
+        <v>2778</v>
       </c>
       <c r="F129">
-        <f t="shared" si="29"/>
-        <v>3989</v>
+        <f t="shared" si="30"/>
+        <v>3911</v>
       </c>
       <c r="G129" s="2">
-        <f t="shared" si="30"/>
-        <v>29993141</v>
+        <f t="shared" si="31"/>
+        <v>29993311</v>
       </c>
       <c r="H129">
-        <f t="shared" si="31"/>
-        <v>3499</v>
+        <f t="shared" si="32"/>
+        <v>3116</v>
       </c>
       <c r="I129" s="4">
         <f t="shared" si="23"/>
-        <v>3562</v>
+        <v>3004</v>
       </c>
       <c r="K129" s="1">
         <f t="shared" si="13"/>
@@ -17513,15 +17617,15 @@
       </c>
       <c r="N129">
         <f t="shared" si="24"/>
-        <v>2870</v>
+        <v>2778</v>
       </c>
       <c r="O129">
         <f t="shared" si="25"/>
-        <v>3499</v>
+        <v>3116</v>
       </c>
       <c r="P129">
-        <f t="shared" si="26"/>
-        <v>3562</v>
+        <f t="shared" si="27"/>
+        <v>3004</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
@@ -17535,28 +17639,28 @@
         <v>1.6</v>
       </c>
       <c r="D130">
-        <f t="shared" si="27"/>
-        <v>29992758</v>
+        <f t="shared" si="28"/>
+        <v>29992941</v>
       </c>
       <c r="E130">
-        <f t="shared" si="28"/>
-        <v>3014</v>
+        <f t="shared" si="29"/>
+        <v>2916</v>
       </c>
       <c r="F130">
-        <f t="shared" si="29"/>
-        <v>4228</v>
+        <f t="shared" si="30"/>
+        <v>4143</v>
       </c>
       <c r="G130" s="2">
-        <f t="shared" si="30"/>
-        <v>29992758</v>
+        <f t="shared" si="31"/>
+        <v>29992941</v>
       </c>
       <c r="H130">
-        <f t="shared" si="31"/>
-        <v>3790</v>
+        <f t="shared" si="32"/>
+        <v>3354</v>
       </c>
       <c r="I130" s="4">
         <f t="shared" si="23"/>
-        <v>3859</v>
+        <v>3235</v>
       </c>
       <c r="K130" s="1">
         <f t="shared" si="13"/>
@@ -17564,15 +17668,15 @@
       </c>
       <c r="N130">
         <f t="shared" si="24"/>
-        <v>3014</v>
+        <v>2916</v>
       </c>
       <c r="O130">
         <f t="shared" si="25"/>
-        <v>3790</v>
+        <v>3354</v>
       </c>
       <c r="P130">
-        <f t="shared" si="26"/>
-        <v>3859</v>
+        <f t="shared" si="27"/>
+        <v>3235</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
@@ -17586,28 +17690,28 @@
         <v>1.6</v>
       </c>
       <c r="D131">
-        <f t="shared" si="27"/>
-        <v>29992356</v>
+        <f t="shared" si="28"/>
+        <v>29992552</v>
       </c>
       <c r="E131">
-        <f t="shared" si="28"/>
-        <v>3165</v>
+        <f t="shared" si="29"/>
+        <v>3062</v>
       </c>
       <c r="F131">
-        <f t="shared" si="29"/>
-        <v>4479</v>
+        <f t="shared" si="30"/>
+        <v>4386</v>
       </c>
       <c r="G131" s="2">
-        <f t="shared" si="30"/>
-        <v>29992356</v>
+        <f t="shared" si="31"/>
+        <v>29992552</v>
       </c>
       <c r="H131">
-        <f t="shared" si="31"/>
-        <v>4106</v>
+        <f t="shared" si="32"/>
+        <v>3611</v>
       </c>
       <c r="I131" s="4">
         <f t="shared" si="23"/>
-        <v>4180</v>
+        <v>3482</v>
       </c>
       <c r="K131" s="1">
         <f t="shared" si="13"/>
@@ -17615,15 +17719,15 @@
       </c>
       <c r="N131">
         <f t="shared" si="24"/>
-        <v>3165</v>
+        <v>3062</v>
       </c>
       <c r="O131">
         <f t="shared" si="25"/>
-        <v>4106</v>
+        <v>3611</v>
       </c>
       <c r="P131">
-        <f t="shared" si="26"/>
-        <v>4180</v>
+        <f t="shared" si="27"/>
+        <v>3482</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
@@ -17637,28 +17741,28 @@
         <v>1.6</v>
       </c>
       <c r="D132">
-        <f t="shared" si="27"/>
-        <v>29991934</v>
+        <f t="shared" si="28"/>
+        <v>29992144</v>
       </c>
       <c r="E132">
-        <f t="shared" si="28"/>
-        <v>3323</v>
+        <f t="shared" si="29"/>
+        <v>3215</v>
       </c>
       <c r="F132">
-        <f t="shared" si="29"/>
-        <v>4743</v>
+        <f t="shared" si="30"/>
+        <v>4641</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" si="30"/>
-        <v>29991934</v>
+        <f t="shared" si="31"/>
+        <v>29992144</v>
       </c>
       <c r="H132">
-        <f t="shared" si="31"/>
-        <v>4448</v>
+        <f t="shared" si="32"/>
+        <v>3888</v>
       </c>
       <c r="I132" s="4">
         <f t="shared" si="23"/>
-        <v>4528</v>
+        <v>3749</v>
       </c>
       <c r="K132" s="1">
         <f t="shared" si="13"/>
@@ -17666,15 +17770,15 @@
       </c>
       <c r="N132">
         <f t="shared" si="24"/>
-        <v>3323</v>
+        <v>3215</v>
       </c>
       <c r="O132">
         <f t="shared" si="25"/>
-        <v>4448</v>
+        <v>3888</v>
       </c>
       <c r="P132">
-        <f t="shared" si="26"/>
-        <v>4528</v>
+        <f t="shared" si="27"/>
+        <v>3749</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
@@ -17688,28 +17792,28 @@
         <v>1.6</v>
       </c>
       <c r="D133">
-        <f t="shared" ref="D133:D134" si="32">D132-ROUND((C133/$D$2)*D132*(E132/$D$3),0)</f>
-        <v>29991491</v>
+        <f t="shared" ref="D133:D134" si="33">D132-ROUND((C133/$D$2)*D132*(E132/$D$3),0)</f>
+        <v>29991715</v>
       </c>
       <c r="E133">
-        <f t="shared" ref="E133:E134" si="33">E132+ROUND((C133/$D$2)*D132*(E132/$D$3),0)-ROUND(E132/$D$2,0)</f>
-        <v>3489</v>
+        <f t="shared" ref="E133:E134" si="34">E132+ROUND((C133/$D$2)*D132*(E132/$D$3),0)-ROUND(E132/$D$2,0)</f>
+        <v>3376</v>
       </c>
       <c r="F133">
-        <f t="shared" ref="F133:F134" si="34">F132+ROUND(E132/$D$2,0)</f>
-        <v>5020</v>
+        <f t="shared" ref="F133:F134" si="35">F132+ROUND(E132/$D$2,0)</f>
+        <v>4909</v>
       </c>
       <c r="G133" s="2">
-        <f t="shared" ref="G133:G134" si="35">D133</f>
-        <v>29991491</v>
+        <f t="shared" ref="G133:G134" si="36">D133</f>
+        <v>29991715</v>
       </c>
       <c r="H133">
-        <f t="shared" ref="H133:H134" si="36">H132+ROUND(($D$1/$D$2)*G132*(H132/$D$3),0)-ROUND(H132/$D$2,0)</f>
-        <v>4818</v>
+        <f t="shared" ref="H133:H134" si="37">H132+ROUND(($D$1/$D$2)*G132*(H132/$D$3),0)-ROUND(H132/$D$2,0)</f>
+        <v>4186</v>
       </c>
       <c r="I133" s="4">
         <f t="shared" si="23"/>
-        <v>4905</v>
+        <v>4037</v>
       </c>
       <c r="K133" s="1">
         <f t="shared" si="13"/>
@@ -17717,15 +17821,15 @@
       </c>
       <c r="N133">
         <f t="shared" si="24"/>
-        <v>3489</v>
+        <v>3376</v>
       </c>
       <c r="O133">
         <f t="shared" si="25"/>
-        <v>4818</v>
+        <v>4186</v>
       </c>
       <c r="P133">
-        <f t="shared" si="26"/>
-        <v>4905</v>
+        <f t="shared" si="27"/>
+        <v>4037</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
@@ -17739,28 +17843,28 @@
         <v>1.6</v>
       </c>
       <c r="D134">
-        <f t="shared" si="32"/>
-        <v>29991026</v>
+        <f t="shared" si="33"/>
+        <v>29991265</v>
       </c>
       <c r="E134">
-        <f t="shared" si="33"/>
-        <v>3663</v>
+        <f t="shared" si="34"/>
+        <v>3545</v>
       </c>
       <c r="F134">
-        <f t="shared" si="34"/>
-        <v>5311</v>
+        <f t="shared" si="35"/>
+        <v>5190</v>
       </c>
       <c r="G134" s="2">
-        <f t="shared" si="35"/>
-        <v>29991026</v>
+        <f t="shared" si="36"/>
+        <v>29991265</v>
       </c>
       <c r="H134">
-        <f t="shared" si="36"/>
-        <v>5219</v>
+        <f t="shared" si="37"/>
+        <v>4507</v>
       </c>
       <c r="I134" s="4">
         <f t="shared" si="23"/>
-        <v>5313</v>
+        <v>4347</v>
       </c>
       <c r="K134" s="1">
         <f t="shared" si="13"/>
@@ -17768,15 +17872,15 @@
       </c>
       <c r="N134">
         <f t="shared" si="24"/>
-        <v>3663</v>
+        <v>3545</v>
       </c>
       <c r="O134">
         <f t="shared" si="25"/>
-        <v>5219</v>
+        <v>4507</v>
       </c>
       <c r="P134">
-        <f t="shared" si="26"/>
-        <v>5313</v>
+        <f t="shared" si="27"/>
+        <v>4347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated and added COVID LOMBARDIA
</commit_message>
<xml_diff>
--- a/COVID_EXCEL/COVID III.xlsx
+++ b/COVID_EXCEL/COVID III.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\u093799\Documents\GitHub\COVID-19\COVID_EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1222E696-8C60-4BA7-BFAE-2F5F2616E3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3450D9-1D26-4483-8A1C-90716973EA4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20880" yWindow="1065" windowWidth="17640" windowHeight="10065" activeTab="1" xr2:uid="{4377578F-4DE2-4D7D-A4C8-86901BC845F0}"/>
+    <workbookView xWindow="1485" yWindow="630" windowWidth="17640" windowHeight="10065" activeTab="1" xr2:uid="{4377578F-4DE2-4D7D-A4C8-86901BC845F0}"/>
   </bookViews>
   <sheets>
     <sheet name="RealData" sheetId="1" r:id="rId1"/>
@@ -662,7 +662,10 @@
                   <c:v>2195</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2323</c:v>
+                  <c:v>2292</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1092,6 +1095,9 @@
                 <c:pt idx="56">
                   <c:v>2292</c:v>
                 </c:pt>
+                <c:pt idx="57">
+                  <c:v>2391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1784,199 +1790,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="65"/>
                 <c:pt idx="0">
-                  <c:v>405</c:v>
+                  <c:v>795</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>407</c:v>
+                  <c:v>797</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>410</c:v>
+                  <c:v>799</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>412</c:v>
+                  <c:v>801</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>415</c:v>
+                  <c:v>803</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>418</c:v>
+                  <c:v>806</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>421</c:v>
+                  <c:v>808</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>424</c:v>
+                  <c:v>811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>428</c:v>
+                  <c:v>814</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>432</c:v>
+                  <c:v>817</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>437</c:v>
+                  <c:v>821</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>442</c:v>
+                  <c:v>824</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>447</c:v>
+                  <c:v>828</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>452</c:v>
+                  <c:v>832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>457</c:v>
+                  <c:v>836</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>463</c:v>
+                  <c:v>841</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>470</c:v>
+                  <c:v>846</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>477</c:v>
+                  <c:v>851</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>485</c:v>
+                  <c:v>857</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>494</c:v>
+                  <c:v>864</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>504</c:v>
+                  <c:v>871</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>515</c:v>
+                  <c:v>879</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>525</c:v>
+                  <c:v>887</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>536</c:v>
+                  <c:v>896</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>549</c:v>
+                  <c:v>906</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>563</c:v>
+                  <c:v>917</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>578</c:v>
+                  <c:v>928</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>594</c:v>
+                  <c:v>940</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>612</c:v>
+                  <c:v>953</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>631</c:v>
+                  <c:v>967</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>651</c:v>
+                  <c:v>982</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>672</c:v>
+                  <c:v>998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>695</c:v>
+                  <c:v>1015</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>719</c:v>
+                  <c:v>1033</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>746</c:v>
+                  <c:v>1054</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>775</c:v>
+                  <c:v>1076</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>806</c:v>
+                  <c:v>1099</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>840</c:v>
+                  <c:v>1124</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>876</c:v>
+                  <c:v>1151</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>915</c:v>
+                  <c:v>1180</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>957</c:v>
+                  <c:v>1212</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1002</c:v>
+                  <c:v>1246</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1051</c:v>
+                  <c:v>1283</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1104</c:v>
+                  <c:v>1323</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1161</c:v>
+                  <c:v>1366</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1222</c:v>
+                  <c:v>1412</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1288</c:v>
+                  <c:v>1462</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1359</c:v>
+                  <c:v>1516</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1436</c:v>
+                  <c:v>1574</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1518</c:v>
+                  <c:v>1636</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1607</c:v>
+                  <c:v>1703</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1703</c:v>
+                  <c:v>1776</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1806</c:v>
+                  <c:v>1854</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1918</c:v>
+                  <c:v>1939</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2039</c:v>
+                  <c:v>2030</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2169</c:v>
+                  <c:v>2129</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2309</c:v>
+                  <c:v>2235</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2461</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2625</c:v>
+                  <c:v>2474</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2801</c:v>
+                  <c:v>2607</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2991</c:v>
+                  <c:v>2751</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3195</c:v>
+                  <c:v>2906</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3415</c:v>
+                  <c:v>3073</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3653</c:v>
+                  <c:v>3254</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3910</c:v>
+                  <c:v>3448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3067,7 +3073,10 @@
                   <c:v>2195</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2323</c:v>
+                  <c:v>2292</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3882,6 +3891,9 @@
                 </c:pt>
                 <c:pt idx="120">
                   <c:v>2292</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4970,7 +4982,10 @@
                   <c:v>2195</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2323</c:v>
+                  <c:v>2292</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5768,6 +5783,9 @@
                 <c:pt idx="120">
                   <c:v>2292</c:v>
                 </c:pt>
+                <c:pt idx="121">
+                  <c:v>2391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6205,25 +6223,25 @@
                   <c:v>2195</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2323</c:v>
+                  <c:v>2292</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2458</c:v>
+                  <c:v>2393</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2601</c:v>
+                  <c:v>2499</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2752</c:v>
+                  <c:v>2610</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2913</c:v>
+                  <c:v>2725</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>3083</c:v>
+                  <c:v>2816</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>3263</c:v>
+                  <c:v>2909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7333,7 +7351,10 @@
                   <c:v>2195</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2323</c:v>
+                  <c:v>2292</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8152,6 +8173,9 @@
                 <c:pt idx="120">
                   <c:v>2292</c:v>
                 </c:pt>
+                <c:pt idx="121">
+                  <c:v>2391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8610,46 +8634,46 @@
                   <c:v>2195</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2323</c:v>
+                  <c:v>2292</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2458</c:v>
+                  <c:v>2393</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2601</c:v>
+                  <c:v>2499</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2752</c:v>
+                  <c:v>2610</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2913</c:v>
+                  <c:v>2725</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>3083</c:v>
+                  <c:v>2816</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>3263</c:v>
+                  <c:v>2909</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>3426</c:v>
+                  <c:v>3006</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>3597</c:v>
+                  <c:v>3106</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>3777</c:v>
+                  <c:v>3209</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>3966</c:v>
+                  <c:v>3316</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>4164</c:v>
+                  <c:v>3427</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>4372</c:v>
+                  <c:v>3541</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>4591</c:v>
+                  <c:v>3659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9158,7 +9182,10 @@
                   <c:v>2195</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2323</c:v>
+                  <c:v>2292</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9396,6 +9423,9 @@
                 <c:pt idx="24">
                   <c:v>2292</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>2391</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9800,103 +9830,103 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>695</c:v>
+                  <c:v>1015</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>719</c:v>
+                  <c:v>1033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>746</c:v>
+                  <c:v>1054</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>775</c:v>
+                  <c:v>1076</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>806</c:v>
+                  <c:v>1099</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>840</c:v>
+                  <c:v>1124</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>876</c:v>
+                  <c:v>1151</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>915</c:v>
+                  <c:v>1180</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>957</c:v>
+                  <c:v>1212</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1002</c:v>
+                  <c:v>1246</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1051</c:v>
+                  <c:v>1283</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1104</c:v>
+                  <c:v>1323</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1161</c:v>
+                  <c:v>1366</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1222</c:v>
+                  <c:v>1412</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1288</c:v>
+                  <c:v>1462</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1359</c:v>
+                  <c:v>1516</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1436</c:v>
+                  <c:v>1574</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1518</c:v>
+                  <c:v>1636</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1607</c:v>
+                  <c:v>1703</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1703</c:v>
+                  <c:v>1776</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1806</c:v>
+                  <c:v>1854</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1918</c:v>
+                  <c:v>1939</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2039</c:v>
+                  <c:v>2030</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2169</c:v>
+                  <c:v>2129</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2309</c:v>
+                  <c:v>2235</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2461</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2625</c:v>
+                  <c:v>2474</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2801</c:v>
+                  <c:v>2607</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2991</c:v>
+                  <c:v>2751</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3195</c:v>
+                  <c:v>2906</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3415</c:v>
+                  <c:v>3073</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3653</c:v>
+                  <c:v>3254</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3910</c:v>
+                  <c:v>3448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23638,10 +23668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ECC772-9D54-48D6-A63B-745C3F43084A}">
-  <dimension ref="A2:K123"/>
+  <dimension ref="A2:K124"/>
   <sheetViews>
     <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+      <selection activeCell="A123" sqref="A123:A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24632,6 +24662,14 @@
         <v>2292</v>
       </c>
     </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>44140</v>
+      </c>
+      <c r="B124">
+        <v>2391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24642,8 +24680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF8076A-EB14-4DFF-97BA-E5541A25D5B9}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C112" workbookViewId="0">
-      <selection activeCell="Q113" sqref="Q113:Q126"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24660,7 +24698,7 @@
         <v>1.94</v>
       </c>
       <c r="E1">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -26909,7 +26947,7 @@
         <v>12</v>
       </c>
       <c r="J54" s="8">
-        <v>385</v>
+        <v>780</v>
       </c>
       <c r="K54" s="1">
         <f t="shared" si="1"/>
@@ -26929,7 +26967,7 @@
       </c>
       <c r="P54">
         <f>J54</f>
-        <v>385</v>
+        <v>780</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -26968,7 +27006,7 @@
       </c>
       <c r="J55" s="8">
         <f>J54+ROUND(($E$1/$D$2)*G54*(I54/$D$3),0)-ROUND(I54/$D$2,0)</f>
-        <v>386</v>
+        <v>781</v>
       </c>
       <c r="K55" s="1">
         <f t="shared" si="1"/>
@@ -26988,7 +27026,7 @@
       </c>
       <c r="P55">
         <f t="shared" ref="P55:P118" si="12">J55</f>
-        <v>386</v>
+        <v>781</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -27027,7 +27065,7 @@
       </c>
       <c r="J56" s="8">
         <f t="shared" ref="J56:J119" si="14">J55+ROUND(($E$1/$D$2)*G55*(I55/$D$3),0)-ROUND(I55/$D$2,0)</f>
-        <v>387</v>
+        <v>782</v>
       </c>
       <c r="K56" s="1">
         <f t="shared" si="1"/>
@@ -27047,7 +27085,7 @@
       </c>
       <c r="P56">
         <f t="shared" si="12"/>
-        <v>387</v>
+        <v>782</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -27086,7 +27124,7 @@
       </c>
       <c r="J57" s="8">
         <f t="shared" si="14"/>
-        <v>388</v>
+        <v>783</v>
       </c>
       <c r="K57" s="1">
         <f t="shared" si="1"/>
@@ -27106,7 +27144,7 @@
       </c>
       <c r="P57">
         <f t="shared" si="12"/>
-        <v>388</v>
+        <v>783</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -27145,7 +27183,7 @@
       </c>
       <c r="J58" s="8">
         <f t="shared" si="14"/>
-        <v>389</v>
+        <v>784</v>
       </c>
       <c r="K58" s="1">
         <f t="shared" si="1"/>
@@ -27165,7 +27203,7 @@
       </c>
       <c r="P58">
         <f t="shared" si="12"/>
-        <v>389</v>
+        <v>784</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -27204,7 +27242,7 @@
       </c>
       <c r="J59" s="8">
         <f t="shared" si="14"/>
-        <v>390</v>
+        <v>785</v>
       </c>
       <c r="K59" s="1">
         <f t="shared" si="1"/>
@@ -27224,7 +27262,7 @@
       </c>
       <c r="P59">
         <f t="shared" si="12"/>
-        <v>390</v>
+        <v>785</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -27263,7 +27301,7 @@
       </c>
       <c r="J60" s="8">
         <f t="shared" si="14"/>
-        <v>391</v>
+        <v>785</v>
       </c>
       <c r="K60" s="1">
         <f t="shared" si="1"/>
@@ -27283,7 +27321,7 @@
       </c>
       <c r="P60">
         <f t="shared" si="12"/>
-        <v>391</v>
+        <v>785</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -27322,7 +27360,7 @@
       </c>
       <c r="J61" s="8">
         <f t="shared" si="14"/>
-        <v>392</v>
+        <v>785</v>
       </c>
       <c r="K61" s="1">
         <f t="shared" si="1"/>
@@ -27342,7 +27380,7 @@
       </c>
       <c r="P61">
         <f t="shared" si="12"/>
-        <v>392</v>
+        <v>785</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -27381,7 +27419,7 @@
       </c>
       <c r="J62" s="8">
         <f t="shared" si="14"/>
-        <v>393</v>
+        <v>786</v>
       </c>
       <c r="K62" s="1">
         <f t="shared" si="1"/>
@@ -27401,7 +27439,7 @@
       </c>
       <c r="P62">
         <f t="shared" si="12"/>
-        <v>393</v>
+        <v>786</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -27440,7 +27478,7 @@
       </c>
       <c r="J63" s="8">
         <f t="shared" si="14"/>
-        <v>394</v>
+        <v>787</v>
       </c>
       <c r="K63" s="1">
         <f t="shared" si="1"/>
@@ -27460,7 +27498,7 @@
       </c>
       <c r="P63">
         <f t="shared" si="12"/>
-        <v>394</v>
+        <v>787</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
@@ -27499,7 +27537,7 @@
       </c>
       <c r="J64" s="8">
         <f t="shared" si="14"/>
-        <v>395</v>
+        <v>788</v>
       </c>
       <c r="K64" s="1">
         <f t="shared" si="1"/>
@@ -27519,7 +27557,7 @@
       </c>
       <c r="P64">
         <f t="shared" si="12"/>
-        <v>395</v>
+        <v>788</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -27558,7 +27596,7 @@
       </c>
       <c r="J65" s="8">
         <f t="shared" si="14"/>
-        <v>396</v>
+        <v>789</v>
       </c>
       <c r="K65" s="1">
         <f t="shared" si="1"/>
@@ -27578,7 +27616,7 @@
       </c>
       <c r="P65">
         <f t="shared" si="12"/>
-        <v>396</v>
+        <v>789</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -27617,7 +27655,7 @@
       </c>
       <c r="J66" s="8">
         <f t="shared" si="14"/>
-        <v>398</v>
+        <v>790</v>
       </c>
       <c r="K66" s="1">
         <f t="shared" si="1"/>
@@ -27637,7 +27675,7 @@
       </c>
       <c r="P66">
         <f t="shared" si="12"/>
-        <v>398</v>
+        <v>790</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -27676,7 +27714,7 @@
       </c>
       <c r="J67" s="8">
         <f t="shared" si="14"/>
-        <v>400</v>
+        <v>792</v>
       </c>
       <c r="K67" s="1">
         <f t="shared" si="1"/>
@@ -27696,7 +27734,7 @@
       </c>
       <c r="P67">
         <f t="shared" si="12"/>
-        <v>400</v>
+        <v>792</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -27735,7 +27773,7 @@
       </c>
       <c r="J68" s="8">
         <f t="shared" si="14"/>
-        <v>401</v>
+        <v>793</v>
       </c>
       <c r="K68" s="1">
         <f t="shared" si="1"/>
@@ -27755,7 +27793,7 @@
       </c>
       <c r="P68">
         <f t="shared" si="12"/>
-        <v>401</v>
+        <v>793</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -27794,7 +27832,7 @@
       </c>
       <c r="J69" s="8">
         <f t="shared" si="14"/>
-        <v>403</v>
+        <v>794</v>
       </c>
       <c r="K69" s="1">
         <f t="shared" si="1"/>
@@ -27814,7 +27852,7 @@
       </c>
       <c r="P69">
         <f t="shared" si="12"/>
-        <v>403</v>
+        <v>794</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -27853,7 +27891,7 @@
       </c>
       <c r="J70" s="8">
         <f t="shared" si="14"/>
-        <v>405</v>
+        <v>795</v>
       </c>
       <c r="K70" s="1">
         <f t="shared" si="1"/>
@@ -27873,7 +27911,7 @@
       </c>
       <c r="P70">
         <f t="shared" si="12"/>
-        <v>405</v>
+        <v>795</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -27912,7 +27950,7 @@
       </c>
       <c r="J71" s="8">
         <f t="shared" si="14"/>
-        <v>407</v>
+        <v>797</v>
       </c>
       <c r="K71" s="1">
         <f t="shared" ref="K71:K134" si="15">A71</f>
@@ -27932,7 +27970,7 @@
       </c>
       <c r="P71">
         <f t="shared" si="12"/>
-        <v>407</v>
+        <v>797</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -27971,7 +28009,7 @@
       </c>
       <c r="J72" s="8">
         <f t="shared" si="14"/>
-        <v>410</v>
+        <v>799</v>
       </c>
       <c r="K72" s="1">
         <f t="shared" si="15"/>
@@ -27991,7 +28029,7 @@
       </c>
       <c r="P72">
         <f t="shared" si="12"/>
-        <v>410</v>
+        <v>799</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -28030,7 +28068,7 @@
       </c>
       <c r="J73" s="8">
         <f t="shared" si="14"/>
-        <v>412</v>
+        <v>801</v>
       </c>
       <c r="K73" s="1">
         <f t="shared" si="15"/>
@@ -28050,7 +28088,7 @@
       </c>
       <c r="P73">
         <f t="shared" si="12"/>
-        <v>412</v>
+        <v>801</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -28089,7 +28127,7 @@
       </c>
       <c r="J74" s="8">
         <f t="shared" si="14"/>
-        <v>415</v>
+        <v>803</v>
       </c>
       <c r="K74" s="1">
         <f t="shared" si="15"/>
@@ -28109,7 +28147,7 @@
       </c>
       <c r="P74">
         <f t="shared" si="12"/>
-        <v>415</v>
+        <v>803</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -28148,7 +28186,7 @@
       </c>
       <c r="J75" s="8">
         <f t="shared" si="14"/>
-        <v>418</v>
+        <v>806</v>
       </c>
       <c r="K75" s="1">
         <f t="shared" si="15"/>
@@ -28168,7 +28206,7 @@
       </c>
       <c r="P75">
         <f t="shared" si="12"/>
-        <v>418</v>
+        <v>806</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -28207,7 +28245,7 @@
       </c>
       <c r="J76" s="8">
         <f t="shared" si="14"/>
-        <v>421</v>
+        <v>808</v>
       </c>
       <c r="K76" s="1">
         <f t="shared" si="15"/>
@@ -28227,7 +28265,7 @@
       </c>
       <c r="P76">
         <f t="shared" si="12"/>
-        <v>421</v>
+        <v>808</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -28266,7 +28304,7 @@
       </c>
       <c r="J77" s="8">
         <f t="shared" si="14"/>
-        <v>424</v>
+        <v>811</v>
       </c>
       <c r="K77" s="1">
         <f t="shared" si="15"/>
@@ -28286,7 +28324,7 @@
       </c>
       <c r="P77">
         <f t="shared" si="12"/>
-        <v>424</v>
+        <v>811</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -28325,7 +28363,7 @@
       </c>
       <c r="J78" s="8">
         <f t="shared" si="14"/>
-        <v>428</v>
+        <v>814</v>
       </c>
       <c r="K78" s="1">
         <f t="shared" si="15"/>
@@ -28345,7 +28383,7 @@
       </c>
       <c r="P78">
         <f t="shared" si="12"/>
-        <v>428</v>
+        <v>814</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -28384,7 +28422,7 @@
       </c>
       <c r="J79" s="8">
         <f t="shared" si="14"/>
-        <v>432</v>
+        <v>817</v>
       </c>
       <c r="K79" s="1">
         <f t="shared" si="15"/>
@@ -28404,7 +28442,7 @@
       </c>
       <c r="P79">
         <f t="shared" si="12"/>
-        <v>432</v>
+        <v>817</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -28443,7 +28481,7 @@
       </c>
       <c r="J80" s="8">
         <f t="shared" si="14"/>
-        <v>437</v>
+        <v>821</v>
       </c>
       <c r="K80" s="1">
         <f t="shared" si="15"/>
@@ -28463,7 +28501,7 @@
       </c>
       <c r="P80">
         <f t="shared" si="12"/>
-        <v>437</v>
+        <v>821</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -28502,7 +28540,7 @@
       </c>
       <c r="J81" s="8">
         <f t="shared" si="14"/>
-        <v>442</v>
+        <v>824</v>
       </c>
       <c r="K81" s="1">
         <f t="shared" si="15"/>
@@ -28522,7 +28560,7 @@
       </c>
       <c r="P81">
         <f t="shared" si="12"/>
-        <v>442</v>
+        <v>824</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -28561,7 +28599,7 @@
       </c>
       <c r="J82" s="8">
         <f t="shared" si="14"/>
-        <v>447</v>
+        <v>828</v>
       </c>
       <c r="K82" s="1">
         <f t="shared" si="15"/>
@@ -28581,7 +28619,7 @@
       </c>
       <c r="P82">
         <f t="shared" si="12"/>
-        <v>447</v>
+        <v>828</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -28620,7 +28658,7 @@
       </c>
       <c r="J83" s="8">
         <f t="shared" si="14"/>
-        <v>452</v>
+        <v>832</v>
       </c>
       <c r="K83" s="1">
         <f t="shared" si="15"/>
@@ -28640,7 +28678,7 @@
       </c>
       <c r="P83">
         <f t="shared" si="12"/>
-        <v>452</v>
+        <v>832</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -28679,7 +28717,7 @@
       </c>
       <c r="J84" s="8">
         <f t="shared" si="14"/>
-        <v>457</v>
+        <v>836</v>
       </c>
       <c r="K84" s="1">
         <f t="shared" si="15"/>
@@ -28699,7 +28737,7 @@
       </c>
       <c r="P84">
         <f t="shared" si="12"/>
-        <v>457</v>
+        <v>836</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -28738,7 +28776,7 @@
       </c>
       <c r="J85" s="8">
         <f t="shared" si="14"/>
-        <v>463</v>
+        <v>841</v>
       </c>
       <c r="K85" s="1">
         <f t="shared" si="15"/>
@@ -28758,7 +28796,7 @@
       </c>
       <c r="P85">
         <f t="shared" si="12"/>
-        <v>463</v>
+        <v>841</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -28797,7 +28835,7 @@
       </c>
       <c r="J86" s="8">
         <f t="shared" si="14"/>
-        <v>470</v>
+        <v>846</v>
       </c>
       <c r="K86" s="1">
         <f t="shared" si="15"/>
@@ -28817,7 +28855,7 @@
       </c>
       <c r="P86">
         <f t="shared" si="12"/>
-        <v>470</v>
+        <v>846</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
@@ -28856,7 +28894,7 @@
       </c>
       <c r="J87" s="8">
         <f t="shared" si="14"/>
-        <v>477</v>
+        <v>851</v>
       </c>
       <c r="K87" s="1">
         <f t="shared" si="15"/>
@@ -28876,7 +28914,7 @@
       </c>
       <c r="P87">
         <f t="shared" si="12"/>
-        <v>477</v>
+        <v>851</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
@@ -28915,7 +28953,7 @@
       </c>
       <c r="J88" s="8">
         <f t="shared" si="14"/>
-        <v>485</v>
+        <v>857</v>
       </c>
       <c r="K88" s="1">
         <f t="shared" si="15"/>
@@ -28935,7 +28973,7 @@
       </c>
       <c r="P88">
         <f t="shared" si="12"/>
-        <v>485</v>
+        <v>857</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
@@ -28974,7 +29012,7 @@
       </c>
       <c r="J89" s="8">
         <f t="shared" si="14"/>
-        <v>494</v>
+        <v>864</v>
       </c>
       <c r="K89" s="1">
         <f t="shared" si="15"/>
@@ -28994,7 +29032,7 @@
       </c>
       <c r="P89">
         <f t="shared" si="12"/>
-        <v>494</v>
+        <v>864</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -29033,7 +29071,7 @@
       </c>
       <c r="J90" s="8">
         <f t="shared" si="14"/>
-        <v>504</v>
+        <v>871</v>
       </c>
       <c r="K90" s="1">
         <f t="shared" si="15"/>
@@ -29053,7 +29091,7 @@
       </c>
       <c r="P90">
         <f t="shared" si="12"/>
-        <v>504</v>
+        <v>871</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -29092,7 +29130,7 @@
       </c>
       <c r="J91" s="8">
         <f t="shared" si="14"/>
-        <v>515</v>
+        <v>879</v>
       </c>
       <c r="K91" s="1">
         <f t="shared" si="15"/>
@@ -29112,7 +29150,7 @@
       </c>
       <c r="P91">
         <f t="shared" si="12"/>
-        <v>515</v>
+        <v>879</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -29151,7 +29189,7 @@
       </c>
       <c r="J92" s="8">
         <f t="shared" si="14"/>
-        <v>525</v>
+        <v>887</v>
       </c>
       <c r="K92" s="1">
         <f t="shared" si="15"/>
@@ -29171,7 +29209,7 @@
       </c>
       <c r="P92">
         <f t="shared" si="12"/>
-        <v>525</v>
+        <v>887</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -29210,7 +29248,7 @@
       </c>
       <c r="J93" s="8">
         <f t="shared" si="14"/>
-        <v>536</v>
+        <v>896</v>
       </c>
       <c r="K93" s="1">
         <f t="shared" si="15"/>
@@ -29230,7 +29268,7 @@
       </c>
       <c r="P93">
         <f t="shared" si="12"/>
-        <v>536</v>
+        <v>896</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -29269,7 +29307,7 @@
       </c>
       <c r="J94" s="8">
         <f t="shared" si="14"/>
-        <v>549</v>
+        <v>906</v>
       </c>
       <c r="K94" s="1">
         <f t="shared" si="15"/>
@@ -29289,7 +29327,7 @@
       </c>
       <c r="P94">
         <f t="shared" si="12"/>
-        <v>549</v>
+        <v>906</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -29328,7 +29366,7 @@
       </c>
       <c r="J95" s="8">
         <f t="shared" si="14"/>
-        <v>563</v>
+        <v>917</v>
       </c>
       <c r="K95" s="1">
         <f t="shared" si="15"/>
@@ -29348,7 +29386,7 @@
       </c>
       <c r="P95">
         <f t="shared" si="12"/>
-        <v>563</v>
+        <v>917</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -29387,7 +29425,7 @@
       </c>
       <c r="J96" s="8">
         <f t="shared" si="14"/>
-        <v>578</v>
+        <v>928</v>
       </c>
       <c r="K96" s="1">
         <f t="shared" si="15"/>
@@ -29407,7 +29445,7 @@
       </c>
       <c r="P96">
         <f t="shared" si="12"/>
-        <v>578</v>
+        <v>928</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -29446,7 +29484,7 @@
       </c>
       <c r="J97" s="8">
         <f t="shared" si="14"/>
-        <v>594</v>
+        <v>940</v>
       </c>
       <c r="K97" s="1">
         <f t="shared" si="15"/>
@@ -29466,7 +29504,7 @@
       </c>
       <c r="P97">
         <f t="shared" si="12"/>
-        <v>594</v>
+        <v>940</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -29505,7 +29543,7 @@
       </c>
       <c r="J98" s="8">
         <f t="shared" si="14"/>
-        <v>612</v>
+        <v>953</v>
       </c>
       <c r="K98" s="1">
         <f t="shared" si="15"/>
@@ -29525,7 +29563,7 @@
       </c>
       <c r="P98">
         <f t="shared" si="12"/>
-        <v>612</v>
+        <v>953</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
@@ -29564,7 +29602,7 @@
       </c>
       <c r="J99" s="8">
         <f t="shared" si="14"/>
-        <v>631</v>
+        <v>967</v>
       </c>
       <c r="K99" s="1">
         <f t="shared" si="15"/>
@@ -29584,7 +29622,7 @@
       </c>
       <c r="P99">
         <f t="shared" si="12"/>
-        <v>631</v>
+        <v>967</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
@@ -29623,7 +29661,7 @@
       </c>
       <c r="J100" s="8">
         <f t="shared" si="14"/>
-        <v>651</v>
+        <v>982</v>
       </c>
       <c r="K100" s="1">
         <f t="shared" si="15"/>
@@ -29643,7 +29681,7 @@
       </c>
       <c r="P100">
         <f t="shared" si="12"/>
-        <v>651</v>
+        <v>982</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
@@ -29682,7 +29720,7 @@
       </c>
       <c r="J101" s="8">
         <f t="shared" si="14"/>
-        <v>672</v>
+        <v>998</v>
       </c>
       <c r="K101" s="1">
         <f t="shared" si="15"/>
@@ -29702,7 +29740,7 @@
       </c>
       <c r="P101">
         <f t="shared" si="12"/>
-        <v>672</v>
+        <v>998</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
@@ -29741,7 +29779,7 @@
       </c>
       <c r="J102" s="8">
         <f t="shared" si="14"/>
-        <v>695</v>
+        <v>1015</v>
       </c>
       <c r="K102" s="1">
         <f t="shared" si="15"/>
@@ -29761,7 +29799,7 @@
       </c>
       <c r="P102">
         <f t="shared" si="12"/>
-        <v>695</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
@@ -29800,7 +29838,7 @@
       </c>
       <c r="J103" s="8">
         <f t="shared" si="14"/>
-        <v>719</v>
+        <v>1033</v>
       </c>
       <c r="K103" s="1">
         <f t="shared" si="15"/>
@@ -29820,7 +29858,7 @@
       </c>
       <c r="P103">
         <f t="shared" si="12"/>
-        <v>719</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
@@ -29859,7 +29897,7 @@
       </c>
       <c r="J104" s="8">
         <f t="shared" si="14"/>
-        <v>746</v>
+        <v>1054</v>
       </c>
       <c r="K104" s="1">
         <f t="shared" si="15"/>
@@ -29879,7 +29917,7 @@
       </c>
       <c r="P104">
         <f t="shared" si="12"/>
-        <v>746</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -29918,7 +29956,7 @@
       </c>
       <c r="J105" s="8">
         <f t="shared" si="14"/>
-        <v>775</v>
+        <v>1076</v>
       </c>
       <c r="K105" s="1">
         <f t="shared" si="15"/>
@@ -29938,7 +29976,7 @@
       </c>
       <c r="P105">
         <f t="shared" si="12"/>
-        <v>775</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -29977,7 +30015,7 @@
       </c>
       <c r="J106" s="8">
         <f t="shared" si="14"/>
-        <v>806</v>
+        <v>1099</v>
       </c>
       <c r="K106" s="1">
         <f t="shared" si="15"/>
@@ -29997,7 +30035,7 @@
       </c>
       <c r="P106">
         <f t="shared" si="12"/>
-        <v>806</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
@@ -30036,7 +30074,7 @@
       </c>
       <c r="J107" s="8">
         <f t="shared" si="14"/>
-        <v>840</v>
+        <v>1124</v>
       </c>
       <c r="K107" s="1">
         <f t="shared" si="15"/>
@@ -30056,7 +30094,7 @@
       </c>
       <c r="P107">
         <f t="shared" si="12"/>
-        <v>840</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
@@ -30095,7 +30133,7 @@
       </c>
       <c r="J108" s="8">
         <f t="shared" si="14"/>
-        <v>876</v>
+        <v>1151</v>
       </c>
       <c r="K108" s="1">
         <f t="shared" si="15"/>
@@ -30115,7 +30153,7 @@
       </c>
       <c r="P108">
         <f t="shared" si="12"/>
-        <v>876</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -30154,7 +30192,7 @@
       </c>
       <c r="J109" s="8">
         <f t="shared" si="14"/>
-        <v>915</v>
+        <v>1180</v>
       </c>
       <c r="K109" s="1">
         <f t="shared" si="15"/>
@@ -30174,7 +30212,7 @@
       </c>
       <c r="P109">
         <f t="shared" si="12"/>
-        <v>915</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -30213,7 +30251,7 @@
       </c>
       <c r="J110" s="8">
         <f t="shared" si="14"/>
-        <v>957</v>
+        <v>1212</v>
       </c>
       <c r="K110" s="1">
         <f t="shared" si="15"/>
@@ -30233,7 +30271,7 @@
       </c>
       <c r="P110">
         <f t="shared" si="12"/>
-        <v>957</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
@@ -30272,7 +30310,7 @@
       </c>
       <c r="J111" s="8">
         <f t="shared" si="14"/>
-        <v>1002</v>
+        <v>1246</v>
       </c>
       <c r="K111" s="1">
         <f t="shared" si="15"/>
@@ -30292,7 +30330,7 @@
       </c>
       <c r="P111">
         <f t="shared" si="12"/>
-        <v>1002</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
@@ -30331,7 +30369,7 @@
       </c>
       <c r="J112" s="8">
         <f t="shared" si="14"/>
-        <v>1051</v>
+        <v>1283</v>
       </c>
       <c r="K112" s="1">
         <f t="shared" si="15"/>
@@ -30351,7 +30389,7 @@
       </c>
       <c r="P112">
         <f t="shared" si="12"/>
-        <v>1051</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
@@ -30390,7 +30428,7 @@
       </c>
       <c r="J113" s="8">
         <f t="shared" si="14"/>
-        <v>1104</v>
+        <v>1323</v>
       </c>
       <c r="K113" s="1">
         <f t="shared" si="15"/>
@@ -30410,7 +30448,7 @@
       </c>
       <c r="P113">
         <f t="shared" si="12"/>
-        <v>1104</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
@@ -30449,7 +30487,7 @@
       </c>
       <c r="J114" s="8">
         <f t="shared" si="14"/>
-        <v>1161</v>
+        <v>1366</v>
       </c>
       <c r="K114" s="1">
         <f t="shared" si="15"/>
@@ -30469,7 +30507,7 @@
       </c>
       <c r="P114">
         <f t="shared" si="12"/>
-        <v>1161</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
@@ -30508,7 +30546,7 @@
       </c>
       <c r="J115" s="8">
         <f t="shared" si="14"/>
-        <v>1222</v>
+        <v>1412</v>
       </c>
       <c r="K115" s="1">
         <f t="shared" si="15"/>
@@ -30528,7 +30566,7 @@
       </c>
       <c r="P115">
         <f t="shared" si="12"/>
-        <v>1222</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
@@ -30567,7 +30605,7 @@
       </c>
       <c r="J116" s="8">
         <f t="shared" si="14"/>
-        <v>1288</v>
+        <v>1462</v>
       </c>
       <c r="K116" s="1">
         <f t="shared" si="15"/>
@@ -30587,7 +30625,7 @@
       </c>
       <c r="P116">
         <f t="shared" si="12"/>
-        <v>1288</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -30626,7 +30664,7 @@
       </c>
       <c r="J117" s="8">
         <f t="shared" si="14"/>
-        <v>1359</v>
+        <v>1516</v>
       </c>
       <c r="K117" s="1">
         <f t="shared" si="15"/>
@@ -30646,7 +30684,7 @@
       </c>
       <c r="P117">
         <f t="shared" si="12"/>
-        <v>1359</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
@@ -30685,7 +30723,7 @@
       </c>
       <c r="J118" s="8">
         <f t="shared" si="14"/>
-        <v>1436</v>
+        <v>1574</v>
       </c>
       <c r="K118" s="1">
         <f t="shared" si="15"/>
@@ -30705,7 +30743,7 @@
       </c>
       <c r="P118">
         <f t="shared" si="12"/>
-        <v>1436</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
@@ -30744,7 +30782,7 @@
       </c>
       <c r="J119" s="8">
         <f t="shared" si="14"/>
-        <v>1518</v>
+        <v>1636</v>
       </c>
       <c r="K119" s="1">
         <f t="shared" si="15"/>
@@ -30764,7 +30802,7 @@
       </c>
       <c r="P119">
         <f t="shared" ref="P119:P134" si="30">J119</f>
-        <v>1518</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
@@ -30803,7 +30841,7 @@
       </c>
       <c r="J120" s="8">
         <f t="shared" ref="J120:J134" si="31">J119+ROUND(($E$1/$D$2)*G119*(I119/$D$3),0)-ROUND(I119/$D$2,0)</f>
-        <v>1607</v>
+        <v>1703</v>
       </c>
       <c r="K120" s="1">
         <f t="shared" si="15"/>
@@ -30823,7 +30861,7 @@
       </c>
       <c r="P120">
         <f t="shared" si="30"/>
-        <v>1607</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
@@ -30862,7 +30900,7 @@
       </c>
       <c r="J121" s="8">
         <f t="shared" si="31"/>
-        <v>1703</v>
+        <v>1776</v>
       </c>
       <c r="K121" s="1">
         <f t="shared" si="15"/>
@@ -30882,7 +30920,7 @@
       </c>
       <c r="P121">
         <f t="shared" si="30"/>
-        <v>1703</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
@@ -30921,7 +30959,7 @@
       </c>
       <c r="J122" s="8">
         <f t="shared" si="31"/>
-        <v>1806</v>
+        <v>1854</v>
       </c>
       <c r="K122" s="1">
         <f t="shared" si="15"/>
@@ -30941,7 +30979,7 @@
       </c>
       <c r="P122">
         <f t="shared" si="30"/>
-        <v>1806</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
@@ -30980,7 +31018,7 @@
       </c>
       <c r="J123" s="8">
         <f t="shared" si="31"/>
-        <v>1918</v>
+        <v>1939</v>
       </c>
       <c r="K123" s="1">
         <f t="shared" si="15"/>
@@ -31000,7 +31038,7 @@
       </c>
       <c r="P123">
         <f t="shared" si="30"/>
-        <v>1918</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
@@ -31039,7 +31077,7 @@
       </c>
       <c r="J124" s="8">
         <f t="shared" si="31"/>
-        <v>2039</v>
+        <v>2030</v>
       </c>
       <c r="K124" s="1">
         <f t="shared" si="15"/>
@@ -31059,7 +31097,7 @@
       </c>
       <c r="P124">
         <f t="shared" si="30"/>
-        <v>2039</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -31098,7 +31136,7 @@
       </c>
       <c r="J125" s="8">
         <f t="shared" si="31"/>
-        <v>2169</v>
+        <v>2129</v>
       </c>
       <c r="K125" s="1">
         <f t="shared" si="15"/>
@@ -31122,7 +31160,7 @@
       </c>
       <c r="P125">
         <f t="shared" si="30"/>
-        <v>2169</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
@@ -31133,15 +31171,15 @@
         <v>121</v>
       </c>
       <c r="C126" s="4">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="D126" s="4">
         <f t="shared" si="35"/>
-        <v>59994358</v>
+        <v>59994389</v>
       </c>
       <c r="E126" s="4">
         <f t="shared" si="36"/>
-        <v>2323</v>
+        <v>2292</v>
       </c>
       <c r="F126" s="4">
         <f t="shared" si="37"/>
@@ -31149,7 +31187,7 @@
       </c>
       <c r="G126" s="2">
         <f t="shared" si="38"/>
-        <v>59994358</v>
+        <v>59994389</v>
       </c>
       <c r="H126" s="2">
         <f t="shared" si="39"/>
@@ -31161,7 +31199,7 @@
       </c>
       <c r="J126" s="8">
         <f t="shared" si="31"/>
-        <v>2309</v>
+        <v>2235</v>
       </c>
       <c r="K126" s="3">
         <f t="shared" si="15"/>
@@ -31169,7 +31207,7 @@
       </c>
       <c r="L126" s="4">
         <f t="shared" ref="L126" si="42">E126</f>
-        <v>2323</v>
+        <v>2292</v>
       </c>
       <c r="M126" s="4">
         <f>RealData!B123</f>
@@ -31177,7 +31215,7 @@
       </c>
       <c r="N126" s="4">
         <f t="shared" si="41"/>
-        <v>2323</v>
+        <v>2292</v>
       </c>
       <c r="O126" s="4">
         <f t="shared" si="29"/>
@@ -31185,7 +31223,7 @@
       </c>
       <c r="P126" s="4">
         <f t="shared" si="30"/>
-        <v>2309</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
@@ -31196,23 +31234,23 @@
         <v>122</v>
       </c>
       <c r="C127" s="4">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="D127" s="4">
         <f t="shared" si="35"/>
-        <v>59994029</v>
+        <v>59994097</v>
       </c>
       <c r="E127" s="4">
         <f t="shared" si="36"/>
-        <v>2458</v>
+        <v>2393</v>
       </c>
       <c r="F127" s="4">
         <f t="shared" si="37"/>
-        <v>3513</v>
+        <v>3510</v>
       </c>
       <c r="G127" s="2">
         <f t="shared" si="38"/>
-        <v>59994029</v>
+        <v>59994097</v>
       </c>
       <c r="H127" s="2">
         <f t="shared" si="39"/>
@@ -31224,17 +31262,23 @@
       </c>
       <c r="J127" s="8">
         <f t="shared" si="31"/>
-        <v>2461</v>
+        <v>2350</v>
       </c>
       <c r="K127" s="3">
         <f t="shared" si="15"/>
         <v>44140</v>
       </c>
-      <c r="L127" s="4"/>
-      <c r="M127" s="4"/>
+      <c r="L127" s="4">
+        <f t="shared" ref="L127" si="43">E127</f>
+        <v>2393</v>
+      </c>
+      <c r="M127" s="4">
+        <f>RealData!B124</f>
+        <v>2391</v>
+      </c>
       <c r="N127" s="4">
         <f t="shared" si="41"/>
-        <v>2458</v>
+        <v>2393</v>
       </c>
       <c r="O127" s="4">
         <f t="shared" si="29"/>
@@ -31242,7 +31286,7 @@
       </c>
       <c r="P127" s="4">
         <f t="shared" si="30"/>
-        <v>2461</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
@@ -31253,23 +31297,23 @@
         <v>123</v>
       </c>
       <c r="C128" s="4">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="D128" s="4">
         <f t="shared" si="35"/>
-        <v>59993681</v>
+        <v>59993792</v>
       </c>
       <c r="E128" s="4">
         <f t="shared" si="36"/>
-        <v>2601</v>
+        <v>2499</v>
       </c>
       <c r="F128" s="4">
         <f t="shared" si="37"/>
-        <v>3718</v>
+        <v>3709</v>
       </c>
       <c r="G128" s="2">
         <f t="shared" si="38"/>
-        <v>59993681</v>
+        <v>59993792</v>
       </c>
       <c r="H128" s="2">
         <f t="shared" si="39"/>
@@ -31281,7 +31325,7 @@
       </c>
       <c r="J128" s="8">
         <f t="shared" si="31"/>
-        <v>2625</v>
+        <v>2474</v>
       </c>
       <c r="K128" s="3">
         <f t="shared" si="15"/>
@@ -31291,7 +31335,7 @@
       <c r="M128" s="4"/>
       <c r="N128" s="4">
         <f t="shared" si="41"/>
-        <v>2601</v>
+        <v>2499</v>
       </c>
       <c r="O128" s="4">
         <f t="shared" si="29"/>
@@ -31299,7 +31343,7 @@
       </c>
       <c r="P128" s="4">
         <f t="shared" si="30"/>
-        <v>2625</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
@@ -31310,23 +31354,23 @@
         <v>124</v>
       </c>
       <c r="C129" s="4">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="D129" s="4">
         <f t="shared" si="35"/>
-        <v>59993313</v>
+        <v>59993473</v>
       </c>
       <c r="E129" s="4">
         <f t="shared" si="36"/>
-        <v>2752</v>
+        <v>2610</v>
       </c>
       <c r="F129" s="4">
         <f t="shared" si="37"/>
-        <v>3935</v>
+        <v>3917</v>
       </c>
       <c r="G129" s="2">
         <f t="shared" si="38"/>
-        <v>59993313</v>
+        <v>59993473</v>
       </c>
       <c r="H129" s="2">
         <f t="shared" si="39"/>
@@ -31338,7 +31382,7 @@
       </c>
       <c r="J129" s="8">
         <f t="shared" si="31"/>
-        <v>2801</v>
+        <v>2607</v>
       </c>
       <c r="K129" s="3">
         <f t="shared" si="15"/>
@@ -31348,7 +31392,7 @@
       <c r="M129" s="4"/>
       <c r="N129" s="4">
         <f t="shared" si="41"/>
-        <v>2752</v>
+        <v>2610</v>
       </c>
       <c r="O129" s="4">
         <f t="shared" si="29"/>
@@ -31356,7 +31400,7 @@
       </c>
       <c r="P129" s="4">
         <f t="shared" si="30"/>
-        <v>2801</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
@@ -31367,23 +31411,23 @@
         <v>125</v>
       </c>
       <c r="C130" s="4">
-        <v>1.7</v>
+        <v>1.53</v>
       </c>
       <c r="D130" s="4">
         <f t="shared" si="35"/>
-        <v>59992923</v>
+        <v>59993140</v>
       </c>
       <c r="E130" s="4">
         <f t="shared" si="36"/>
-        <v>2913</v>
+        <v>2725</v>
       </c>
       <c r="F130" s="4">
         <f t="shared" si="37"/>
-        <v>4164</v>
+        <v>4135</v>
       </c>
       <c r="G130" s="2">
         <f t="shared" si="38"/>
-        <v>59992923</v>
+        <v>59993140</v>
       </c>
       <c r="H130" s="2">
         <f t="shared" si="39"/>
@@ -31395,7 +31439,7 @@
       </c>
       <c r="J130" s="8">
         <f t="shared" si="31"/>
-        <v>2991</v>
+        <v>2751</v>
       </c>
       <c r="K130" s="3">
         <f t="shared" si="15"/>
@@ -31405,7 +31449,7 @@
       <c r="M130" s="4"/>
       <c r="N130" s="4">
         <f t="shared" si="41"/>
-        <v>2913</v>
+        <v>2725</v>
       </c>
       <c r="O130" s="4">
         <f t="shared" si="29"/>
@@ -31413,7 +31457,7 @@
       </c>
       <c r="P130" s="4">
         <f t="shared" si="30"/>
-        <v>2991</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
@@ -31424,23 +31468,23 @@
         <v>126</v>
       </c>
       <c r="C131" s="4">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="D131" s="4">
         <f t="shared" si="35"/>
-        <v>59992510</v>
+        <v>59992822</v>
       </c>
       <c r="E131" s="4">
         <f t="shared" si="36"/>
-        <v>3083</v>
+        <v>2816</v>
       </c>
       <c r="F131" s="4">
         <f t="shared" si="37"/>
-        <v>4407</v>
+        <v>4362</v>
       </c>
       <c r="G131" s="2">
         <f t="shared" si="38"/>
-        <v>59992510</v>
+        <v>59992822</v>
       </c>
       <c r="H131" s="2">
         <f t="shared" si="39"/>
@@ -31452,7 +31496,7 @@
       </c>
       <c r="J131" s="8">
         <f t="shared" si="31"/>
-        <v>3195</v>
+        <v>2906</v>
       </c>
       <c r="K131" s="3">
         <f t="shared" si="15"/>
@@ -31462,7 +31506,7 @@
       <c r="M131" s="4"/>
       <c r="N131" s="4">
         <f t="shared" si="41"/>
-        <v>3083</v>
+        <v>2816</v>
       </c>
       <c r="O131" s="4">
         <f t="shared" si="29"/>
@@ -31470,7 +31514,7 @@
       </c>
       <c r="P131" s="4">
         <f t="shared" si="30"/>
-        <v>3195</v>
+        <v>2906</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
@@ -31481,23 +31525,23 @@
         <v>127</v>
       </c>
       <c r="C132" s="4">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="D132" s="4">
         <f t="shared" si="35"/>
-        <v>59992073</v>
+        <v>59992494</v>
       </c>
       <c r="E132" s="4">
         <f t="shared" si="36"/>
-        <v>3263</v>
+        <v>2909</v>
       </c>
       <c r="F132" s="4">
         <f t="shared" si="37"/>
-        <v>4664</v>
+        <v>4597</v>
       </c>
       <c r="G132" s="2">
         <f t="shared" si="38"/>
-        <v>59992073</v>
+        <v>59992494</v>
       </c>
       <c r="H132" s="2">
         <f t="shared" si="39"/>
@@ -31509,7 +31553,7 @@
       </c>
       <c r="J132" s="8">
         <f t="shared" si="31"/>
-        <v>3415</v>
+        <v>3073</v>
       </c>
       <c r="K132" s="3">
         <f t="shared" si="15"/>
@@ -31519,7 +31563,7 @@
       <c r="M132" s="4"/>
       <c r="N132" s="4">
         <f t="shared" si="41"/>
-        <v>3263</v>
+        <v>2909</v>
       </c>
       <c r="O132" s="4">
         <f t="shared" si="29"/>
@@ -31527,7 +31571,7 @@
       </c>
       <c r="P132" s="4">
         <f t="shared" si="30"/>
-        <v>3415</v>
+        <v>3073</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
@@ -31538,26 +31582,26 @@
         <v>128</v>
       </c>
       <c r="C133" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D133" s="10">
-        <f t="shared" ref="D133:D134" si="43">D132-ROUND((C133/$D$2)*D132*(E132/$D$3),0)</f>
-        <v>59991638</v>
+        <f t="shared" ref="D133:D134" si="44">D132-ROUND((C133/$D$2)*D132*(E132/$D$3),0)</f>
+        <v>59992155</v>
       </c>
       <c r="E133" s="10">
-        <f t="shared" ref="E133:E134" si="44">E132+ROUND((C133/$D$2)*D132*(E132/$D$3),0)-ROUND(E132/$D$2,0)</f>
-        <v>3426</v>
+        <f t="shared" ref="E133:E134" si="45">E132+ROUND((C133/$D$2)*D132*(E132/$D$3),0)-ROUND(E132/$D$2,0)</f>
+        <v>3006</v>
       </c>
       <c r="F133" s="10">
-        <f t="shared" ref="F133:F134" si="45">F132+ROUND(E132/$D$2,0)</f>
-        <v>4936</v>
+        <f t="shared" ref="F133:F134" si="46">F132+ROUND(E132/$D$2,0)</f>
+        <v>4839</v>
       </c>
       <c r="G133" s="2">
-        <f t="shared" ref="G133:G134" si="46">D133</f>
-        <v>59991638</v>
+        <f t="shared" ref="G133:G134" si="47">D133</f>
+        <v>59992155</v>
       </c>
       <c r="H133" s="2">
-        <f t="shared" ref="H133:H134" si="47">H132+ROUND(($D$1/$D$2)*G132*(H132/$D$3),0)-ROUND(H132/$D$2,0)</f>
+        <f t="shared" ref="H133:H134" si="48">H132+ROUND(($D$1/$D$2)*G132*(H132/$D$3),0)-ROUND(H132/$D$2,0)</f>
         <v>4403</v>
       </c>
       <c r="I133" s="7">
@@ -31566,7 +31610,7 @@
       </c>
       <c r="J133" s="8">
         <f t="shared" si="31"/>
-        <v>3653</v>
+        <v>3254</v>
       </c>
       <c r="K133" s="9">
         <f t="shared" si="15"/>
@@ -31576,7 +31620,7 @@
       <c r="M133" s="10"/>
       <c r="N133" s="10">
         <f t="shared" si="41"/>
-        <v>3426</v>
+        <v>3006</v>
       </c>
       <c r="O133" s="10">
         <f t="shared" si="29"/>
@@ -31584,7 +31628,7 @@
       </c>
       <c r="P133" s="10">
         <f t="shared" si="30"/>
-        <v>3653</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
@@ -31595,26 +31639,26 @@
         <v>129</v>
       </c>
       <c r="C134" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D134" s="10">
-        <f t="shared" si="43"/>
-        <v>59991181</v>
+        <f t="shared" si="44"/>
+        <v>59991804</v>
       </c>
       <c r="E134" s="10">
-        <f t="shared" si="44"/>
-        <v>3597</v>
+        <f t="shared" si="45"/>
+        <v>3106</v>
       </c>
       <c r="F134" s="10">
-        <f t="shared" si="45"/>
-        <v>5222</v>
+        <f t="shared" si="46"/>
+        <v>5090</v>
       </c>
       <c r="G134" s="2">
-        <f t="shared" si="46"/>
-        <v>59991181</v>
+        <f t="shared" si="47"/>
+        <v>59991804</v>
       </c>
       <c r="H134" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>4748</v>
       </c>
       <c r="I134" s="7">
@@ -31623,7 +31667,7 @@
       </c>
       <c r="J134" s="8">
         <f t="shared" si="31"/>
-        <v>3910</v>
+        <v>3448</v>
       </c>
       <c r="K134" s="9">
         <f t="shared" si="15"/>
@@ -31633,7 +31677,7 @@
       <c r="M134" s="10"/>
       <c r="N134" s="10">
         <f t="shared" si="41"/>
-        <v>3597</v>
+        <v>3106</v>
       </c>
       <c r="O134" s="10">
         <f t="shared" si="29"/>
@@ -31641,7 +31685,7 @@
       </c>
       <c r="P134" s="10">
         <f t="shared" si="30"/>
-        <v>3910</v>
+        <v>3448</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
@@ -31652,53 +31696,53 @@
         <v>130</v>
       </c>
       <c r="C135" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D135" s="10">
-        <f t="shared" ref="D135:D139" si="48">D134-ROUND((C135/$D$2)*D134*(E134/$D$3),0)</f>
-        <v>59990701</v>
+        <f t="shared" ref="D135:D139" si="49">D134-ROUND((C135/$D$2)*D134*(E134/$D$3),0)</f>
+        <v>59991442</v>
       </c>
       <c r="E135" s="10">
-        <f t="shared" ref="E135:E139" si="49">E134+ROUND((C135/$D$2)*D134*(E134/$D$3),0)-ROUND(E134/$D$2,0)</f>
-        <v>3777</v>
+        <f t="shared" ref="E135:E139" si="50">E134+ROUND((C135/$D$2)*D134*(E134/$D$3),0)-ROUND(E134/$D$2,0)</f>
+        <v>3209</v>
       </c>
       <c r="F135" s="10">
-        <f t="shared" ref="F135:F139" si="50">F134+ROUND(E134/$D$2,0)</f>
-        <v>5522</v>
+        <f t="shared" ref="F135:F139" si="51">F134+ROUND(E134/$D$2,0)</f>
+        <v>5349</v>
       </c>
       <c r="G135" s="2">
-        <f t="shared" ref="G135:G139" si="51">D135</f>
-        <v>59990701</v>
+        <f t="shared" ref="G135:G139" si="52">D135</f>
+        <v>59991442</v>
       </c>
       <c r="H135" s="2">
-        <f t="shared" ref="H135:H139" si="52">H134+ROUND(($D$1/$D$2)*G134*(H134/$D$3),0)-ROUND(H134/$D$2,0)</f>
+        <f t="shared" ref="H135:H139" si="53">H134+ROUND(($D$1/$D$2)*G134*(H134/$D$3),0)-ROUND(H134/$D$2,0)</f>
         <v>5119</v>
       </c>
       <c r="I135" s="7">
-        <f t="shared" ref="I135:I139" si="53">I134+ROUND(($D$1/$D$2)*G134*(I134/$D$3),0)-ROUND(I134/$D$2,0)</f>
+        <f t="shared" ref="I135:I139" si="54">I134+ROUND(($D$1/$D$2)*G134*(I134/$D$3),0)-ROUND(I134/$D$2,0)</f>
         <v>5119</v>
       </c>
       <c r="J135" s="8">
-        <f t="shared" ref="J135:J139" si="54">J134+ROUND(($E$1/$D$2)*G134*(I134/$D$3),0)-ROUND(I134/$D$2,0)</f>
-        <v>4187</v>
+        <f t="shared" ref="J135:J139" si="55">J134+ROUND(($E$1/$D$2)*G134*(I134/$D$3),0)-ROUND(I134/$D$2,0)</f>
+        <v>3657</v>
       </c>
       <c r="K135" s="9">
-        <f t="shared" ref="K135:K139" si="55">A135</f>
+        <f t="shared" ref="K135:K139" si="56">A135</f>
         <v>44148</v>
       </c>
       <c r="L135" s="10"/>
       <c r="M135" s="10"/>
       <c r="N135" s="10">
-        <f t="shared" ref="N135:N139" si="56">E135</f>
-        <v>3777</v>
+        <f t="shared" ref="N135:N139" si="57">E135</f>
+        <v>3209</v>
       </c>
       <c r="O135" s="10">
-        <f t="shared" ref="O135:O139" si="57">I135</f>
+        <f t="shared" ref="O135:O139" si="58">I135</f>
         <v>5119</v>
       </c>
       <c r="P135" s="10">
-        <f t="shared" ref="P135:P139" si="58">J135</f>
-        <v>4187</v>
+        <f t="shared" ref="P135:P139" si="59">J135</f>
+        <v>3657</v>
       </c>
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
@@ -31709,53 +31753,53 @@
         <v>131</v>
       </c>
       <c r="C136" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D136" s="10">
-        <f t="shared" si="48"/>
-        <v>59990197</v>
+        <f t="shared" si="49"/>
+        <v>59991068</v>
       </c>
       <c r="E136" s="10">
-        <f t="shared" si="49"/>
-        <v>3966</v>
+        <f t="shared" si="50"/>
+        <v>3316</v>
       </c>
       <c r="F136" s="10">
-        <f t="shared" si="50"/>
-        <v>5837</v>
+        <f t="shared" si="51"/>
+        <v>5616</v>
       </c>
       <c r="G136" s="2">
-        <f t="shared" si="51"/>
-        <v>59990197</v>
+        <f t="shared" si="52"/>
+        <v>59991068</v>
       </c>
       <c r="H136" s="2">
-        <f t="shared" si="52"/>
-        <v>5519</v>
-      </c>
-      <c r="I136" s="7">
         <f t="shared" si="53"/>
         <v>5519</v>
       </c>
+      <c r="I136" s="7">
+        <f t="shared" si="54"/>
+        <v>5519</v>
+      </c>
       <c r="J136" s="8">
-        <f t="shared" si="54"/>
-        <v>4485</v>
+        <f t="shared" si="55"/>
+        <v>3883</v>
       </c>
       <c r="K136" s="9">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>44149</v>
       </c>
       <c r="L136" s="10"/>
       <c r="M136" s="10"/>
       <c r="N136" s="10">
-        <f t="shared" si="56"/>
-        <v>3966</v>
+        <f t="shared" si="57"/>
+        <v>3316</v>
       </c>
       <c r="O136" s="10">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>5519</v>
       </c>
       <c r="P136" s="10">
-        <f t="shared" si="58"/>
-        <v>4485</v>
+        <f t="shared" si="59"/>
+        <v>3883</v>
       </c>
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
@@ -31766,53 +31810,53 @@
         <v>132</v>
       </c>
       <c r="C137" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D137" s="10">
-        <f t="shared" si="48"/>
-        <v>59989668</v>
+        <f t="shared" si="49"/>
+        <v>59990681</v>
       </c>
       <c r="E137" s="10">
-        <f t="shared" si="49"/>
-        <v>4164</v>
+        <f t="shared" si="50"/>
+        <v>3427</v>
       </c>
       <c r="F137" s="10">
-        <f t="shared" si="50"/>
-        <v>6168</v>
+        <f t="shared" si="51"/>
+        <v>5892</v>
       </c>
       <c r="G137" s="2">
-        <f t="shared" si="51"/>
-        <v>59989668</v>
+        <f t="shared" si="52"/>
+        <v>59990681</v>
       </c>
       <c r="H137" s="2">
-        <f t="shared" si="52"/>
-        <v>5951</v>
-      </c>
-      <c r="I137" s="7">
         <f t="shared" si="53"/>
         <v>5951</v>
       </c>
+      <c r="I137" s="7">
+        <f t="shared" si="54"/>
+        <v>5951</v>
+      </c>
       <c r="J137" s="8">
-        <f t="shared" si="54"/>
-        <v>4807</v>
+        <f t="shared" si="55"/>
+        <v>4127</v>
       </c>
       <c r="K137" s="9">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>44150</v>
       </c>
       <c r="L137" s="10"/>
       <c r="M137" s="10"/>
       <c r="N137" s="10">
-        <f t="shared" si="56"/>
-        <v>4164</v>
+        <f t="shared" si="57"/>
+        <v>3427</v>
       </c>
       <c r="O137" s="10">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>5951</v>
       </c>
       <c r="P137" s="10">
-        <f t="shared" si="58"/>
-        <v>4807</v>
+        <f t="shared" si="59"/>
+        <v>4127</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
@@ -31823,53 +31867,53 @@
         <v>133</v>
       </c>
       <c r="C138" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D138" s="10">
-        <f t="shared" si="48"/>
-        <v>59989113</v>
+        <f t="shared" si="49"/>
+        <v>59990281</v>
       </c>
       <c r="E138" s="10">
-        <f t="shared" si="49"/>
-        <v>4372</v>
+        <f t="shared" si="50"/>
+        <v>3541</v>
       </c>
       <c r="F138" s="10">
-        <f t="shared" si="50"/>
-        <v>6515</v>
+        <f t="shared" si="51"/>
+        <v>6178</v>
       </c>
       <c r="G138" s="2">
-        <f t="shared" si="51"/>
-        <v>59989113</v>
+        <f t="shared" si="52"/>
+        <v>59990281</v>
       </c>
       <c r="H138" s="2">
-        <f t="shared" si="52"/>
-        <v>6417</v>
-      </c>
-      <c r="I138" s="7">
         <f t="shared" si="53"/>
         <v>6417</v>
       </c>
+      <c r="I138" s="7">
+        <f t="shared" si="54"/>
+        <v>6417</v>
+      </c>
       <c r="J138" s="8">
-        <f t="shared" si="54"/>
-        <v>5154</v>
+        <f t="shared" si="55"/>
+        <v>4390</v>
       </c>
       <c r="K138" s="9">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>44151</v>
       </c>
       <c r="L138" s="10"/>
       <c r="M138" s="10"/>
       <c r="N138" s="10">
-        <f t="shared" si="56"/>
-        <v>4372</v>
+        <f t="shared" si="57"/>
+        <v>3541</v>
       </c>
       <c r="O138" s="10">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>6417</v>
       </c>
       <c r="P138" s="10">
-        <f t="shared" si="58"/>
-        <v>5154</v>
+        <f t="shared" si="59"/>
+        <v>4390</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
@@ -31880,53 +31924,53 @@
         <v>134</v>
       </c>
       <c r="C139" s="10">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D139" s="10">
-        <f t="shared" si="48"/>
-        <v>59988530</v>
+        <f t="shared" si="49"/>
+        <v>59989868</v>
       </c>
       <c r="E139" s="10">
-        <f t="shared" si="49"/>
-        <v>4591</v>
+        <f t="shared" si="50"/>
+        <v>3659</v>
       </c>
       <c r="F139" s="10">
-        <f t="shared" si="50"/>
-        <v>6879</v>
+        <f t="shared" si="51"/>
+        <v>6473</v>
       </c>
       <c r="G139" s="2">
-        <f t="shared" si="51"/>
-        <v>59988530</v>
+        <f t="shared" si="52"/>
+        <v>59989868</v>
       </c>
       <c r="H139" s="2">
-        <f t="shared" si="52"/>
-        <v>6919</v>
-      </c>
-      <c r="I139" s="7">
         <f t="shared" si="53"/>
         <v>6919</v>
       </c>
+      <c r="I139" s="7">
+        <f t="shared" si="54"/>
+        <v>6919</v>
+      </c>
       <c r="J139" s="8">
-        <f t="shared" si="54"/>
-        <v>5528</v>
+        <f t="shared" si="55"/>
+        <v>4673</v>
       </c>
       <c r="K139" s="9">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>44152</v>
       </c>
       <c r="L139" s="10"/>
       <c r="M139" s="10"/>
       <c r="N139" s="10">
-        <f t="shared" si="56"/>
-        <v>4591</v>
+        <f t="shared" si="57"/>
+        <v>3659</v>
       </c>
       <c r="O139" s="10">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>6919</v>
       </c>
       <c r="P139" s="10">
-        <f t="shared" si="58"/>
-        <v>5528</v>
+        <f t="shared" si="59"/>
+        <v>4673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>